<commit_message>
Add "LOG","resource" and "urlTransitionSheetName" fields in "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean" class Add "getSheet(org.apache.poi.ss.usermodel.Workbook,java.lang.String)","getStringCellValue(org.apache.poi.ss.usermodel.Cell,org.apache.poi.ss.usermodel.FormulaEvaluator)" and "putAll(java.util.Map,java.util.Map)" methods in "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean" class Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean.urlTransitionSheetName" property in "configuration.properties" Add "url_transition" sheet in "OtoYakuNoHeyaYomikataJiten.xlsx" Implements "org.springframework.beans.factory.InitializingBean" interface by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean" class
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="url_transition" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="202">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -171,6 +172,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">付録・</t>
     </r>
@@ -179,6 +181,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">φ</t>
     </r>
@@ -187,6 +190,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">の読み方</t>
     </r>
@@ -200,6 +204,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">単位の読み方（１）</t>
     </r>
@@ -208,6 +213,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SI</t>
     </r>
@@ -216,6 +222,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">単位</t>
     </r>
@@ -259,6 +266,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">JR</t>
     </r>
@@ -267,6 +275,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">線　読み方辞典</t>
     </r>
@@ -280,6 +289,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">民営鉄道（</t>
     </r>
@@ -288,6 +298,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">JR</t>
     </r>
@@ -296,6 +307,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">以外）読み方辞典</t>
     </r>
@@ -405,6 +417,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">暦のことば読み方（</t>
     </r>
@@ -413,6 +426,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50</t>
     </r>
@@ -421,6 +435,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">音順）</t>
     </r>
@@ -482,6 +497,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2012</t>
     </r>
@@ -490,6 +506,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年オリンピック日本選手団</t>
     </r>
@@ -503,6 +520,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2014</t>
     </r>
@@ -511,6 +529,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年ソチオリンピック日本選手団</t>
     </r>
@@ -524,6 +543,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2016</t>
     </r>
@@ -532,6 +552,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年リオオリンピック日本選手団</t>
     </r>
@@ -545,6 +566,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">リオ</t>
     </r>
@@ -553,6 +575,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2016</t>
     </r>
@@ -561,6 +584,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年パラリンピック日本選手団</t>
     </r>
@@ -670,6 +694,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ISBN</t>
     </r>
@@ -678,6 +703,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">・</t>
     </r>
@@ -686,6 +712,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">E-mail</t>
     </r>
@@ -694,6 +721,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">・</t>
     </r>
@@ -702,6 +730,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">URL</t>
     </r>
@@ -710,6 +739,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">の読み方</t>
     </r>
@@ -801,6 +831,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">にほんの里</t>
     </r>
@@ -809,6 +840,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">100</t>
     </r>
@@ -817,6 +849,7 @@
         <sz val="10"/>
         <rFont val="Yu Gothic"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">選</t>
     </r>
@@ -865,6 +898,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/tosho-01.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.gsi.go.jp/KIDS/map-sign-tizukigou-h14kigou-itiran.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20211126172558/http://www.gsi.go.jp/KIDS/map-sign-tizukigou-h14kigou-itiran.htm</t>
   </si>
 </sst>
 </file>
@@ -879,6 +918,7 @@
       <sz val="10"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -899,6 +939,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -943,12 +984,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1077,1605 +1122,1605 @@
   </sheetPr>
   <dimension ref="A1:B199"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A187" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="57.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
+      <c r="A67" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
+      <c r="A69" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
+      <c r="A71" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
+      <c r="A73" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
+      <c r="A75" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
+      <c r="A77" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
+      <c r="A79" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
+      <c r="A81" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
+      <c r="A83" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
+      <c r="A85" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
+      <c r="A87" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
+      <c r="A89" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
+      <c r="A91" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
+      <c r="A93" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="n">
+      <c r="A95" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="n">
+      <c r="A97" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="n">
+      <c r="A99" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
+      <c r="A101" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="n">
+      <c r="A103" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="A104" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="n">
+      <c r="A105" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="A106" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="n">
+      <c r="A107" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="n">
+      <c r="A109" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="n">
+      <c r="A111" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="n">
+      <c r="A113" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="n">
+      <c r="A115" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="1" t="s">
+      <c r="A116" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="n">
+      <c r="A117" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="n">
+      <c r="A119" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="n">
+      <c r="A121" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="n">
+      <c r="A123" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="2" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="n">
+      <c r="A125" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="A126" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="n">
+      <c r="A127" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="2" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="A128" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="n">
+      <c r="A129" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="A130" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="n">
+      <c r="A131" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="A132" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="n">
+      <c r="A133" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="2" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+      <c r="A134" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="n">
+      <c r="A135" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="A136" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="n">
+      <c r="A137" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="A138" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="n">
+      <c r="A139" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="A140" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="n">
+      <c r="A141" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="A142" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="n">
+      <c r="A143" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="2" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
+      <c r="A144" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="n">
+      <c r="A145" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="A146" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="n">
+      <c r="A147" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
+      <c r="A148" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="n">
+      <c r="A149" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" s="2" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
+      <c r="A150" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="n">
+      <c r="A151" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
+      <c r="A152" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="n">
+      <c r="A153" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
+      <c r="A154" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" s="2" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="n">
+      <c r="A155" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="2" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
+      <c r="A156" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="n">
+      <c r="A157" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="2" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
+      <c r="A158" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="2" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="n">
+      <c r="A159" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="2" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
+      <c r="A160" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="n">
+      <c r="A161" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
+      <c r="A162" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="n">
+      <c r="A163" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
+      <c r="A164" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="n">
+      <c r="A165" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="2" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
+      <c r="A166" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="n">
+      <c r="A167" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="2" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
+      <c r="A168" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="n">
+      <c r="A169" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="2" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
+      <c r="A170" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="n">
+      <c r="A171" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B171" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
+      <c r="A172" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="n">
+      <c r="A173" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
+      <c r="A174" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B174" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="n">
+      <c r="A175" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B175" s="2" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
+      <c r="A176" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="n">
+      <c r="A177" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
+      <c r="A178" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="n">
+      <c r="A179" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+      <c r="A180" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B180" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="n">
+      <c r="A181" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B181" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+      <c r="A182" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B182" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="n">
+      <c r="A183" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B183" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+      <c r="A184" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B184" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="n">
+      <c r="A185" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" s="2" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+      <c r="A186" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B186" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="n">
+      <c r="A187" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="B187" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
+      <c r="A188" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="1" t="s">
+      <c r="B188" s="2" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="n">
+      <c r="A189" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B189" s="1" t="s">
+      <c r="B189" s="2" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
+      <c r="A190" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B190" s="1" t="s">
+      <c r="B190" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="n">
+      <c r="A191" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B191" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+      <c r="A192" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B192" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="n">
+      <c r="A193" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B193" s="1" t="s">
+      <c r="B193" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
+      <c r="A194" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B194" s="1" t="s">
+      <c r="B194" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="n">
+      <c r="A195" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="B195" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
+      <c r="A196" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B196" s="2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="n">
+      <c r="A197" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B197" s="2" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
+      <c r="A198" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B198" s="1" t="s">
+      <c r="B198" s="2" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="n">
+      <c r="A199" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B199" s="1" t="s">
+      <c r="B199" s="2" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2688,4 +2733,40 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add "linkSheetName" field in "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean" class Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean$IntStringMap" interface Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean.formatCellValue(org.apache.poi.ss.usermodel.DataFormatter,org.apache.poi.ss.usermodel.Cell)" method Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean.linkSheetName" property in "configuration.properties" Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenLinkMapFactoryBean.getObject()" method
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="url_transition" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="link" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="441">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -904,6 +905,1919 @@
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20211126172558/http://www.gsi.go.jp/KIDS/map-sign-tizukigou-h14kigou-itiran.htm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImgSrc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">医学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">病名の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">身体の部位・症状・その他の読み方５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">臨床でよく使われる単位の読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">漢方処方の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">和漢薬・生薬の読み方　総画数順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">１４経絡（けいらく）のツボの読み方　部位別</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈良時代−明治初期の医家人名の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">漢方書籍名の読み方　５０音順　・作者名読み方付</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">厚生省発表の健康被害をおこすダイエット食品読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新型コロナウイルス感染症（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">COVID-19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）関連用語の読み方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">科学</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生物・化学用語の読み方　５０音順　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶の科学用語・農業用語・茶の種類　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">物理用語の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">算数・数学用語 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順　数式記号の読み方へのリンク</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マイデータを整理。物理用語読み方辞典付表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地学用語の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大日本沿岸輿地全図（伊能忠敬の日本地図）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地図学用語に関する読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地理学用語の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">気象用語の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">産業 技術</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">建築設備用語・建築現場用語・木造建築用語 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ロボット・ロボット関係者の読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">記号 単位</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">文章中の符号、数学記号、理科記号、商用記号他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10/19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">付録・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">φ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">の読み方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">単位の読み方（１）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">SI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">単位</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">科学の本を読むために　通産省の冊子より抜粋作成</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">接頭語及び単位一覧　読み方の例あり。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尺貫法などの読み方・古代地方行政区分</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">シーベルト（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ｖ）ベクレル（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ｑ）グレイ（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ｙ）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">マイデータを整理。図・表・グラフ・写真等の読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">数詞・助数詞の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">JR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">線　読み方辞典</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">交通</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">JR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">線名の読み方（地区別）全国駅名の読み方へリンク</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">民営鉄道（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">JR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">以外）読み方辞典</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">私鉄・第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">セクター（社名・路線名）読み方・駅名へリンク</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">高速道路ＪＣＴ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ＩＣ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ＳＡ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ＰＡの読み方　地域別</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">静岡県内（御殿場</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">JCT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">〜三ヶ日</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">JCT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）部分開通</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">都市高速道路の読み方 福岡北九州</t>
+  </si>
+  <si>
+    <t xml:space="preserve">都市高速道路の読み方 首都高速</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/onyak2/tosiko02.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">都市高速道路の読み方 広島</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/onyak2/tosiko03.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">都市高速道路の読み方 阪神</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/onyak2/tosiko04.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">都市高速道路の読み方 名古屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/onyak2/tosiko05.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ＪＨ（日本道路公団）以外の有料道路の読み方　県別</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">政経</t>
+  </si>
+  <si>
+    <t xml:space="preserve">会計・金融・経済・株式・先物取引用語 読み方辞典</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">法律用語の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">歴史</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">検索システム・遺跡</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">・発掘情報・最近報道の遺跡</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">年号（元号）一覧・西暦対照表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">歴代天皇と御陵の読み方・参考に西暦対照表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">昔の職業や職人の読み方が５０音順、遊び心で楽しく。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">文化</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日本の伝統的な色を中心に色名の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日本の伝統的な文様の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">和紙の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ブックデザイナー・イラストレーター・挿画家・写真家など</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">書籍・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">WEB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">等にある編集者・出版関係者</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日本の暦に関する言葉の読み方　項目別</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">暦のことば読み方（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">日本の暦に関する言葉の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">茶道用語　茶人の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">煎茶用語　文人の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">いけばな用語の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">やきもの用語の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">香道用語の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">刀剣用語 読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">アルファベット運動略語　数字を含むスポーツ用語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">相撲用語の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順　</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2012</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年オリンピック日本選手団</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ロンドンオリンピック日本代表選手団　読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2014</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年ソチオリンピック日本選手団</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ソチオリンピック日本代表選手団　読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年リオオリンピック日本選手団</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">リオデジャネイロオリンピック日本選手団</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">リオ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年パラリンピック日本選手団</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">リオ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年パラリンピック日本代表選手団</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">61</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">第</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">62</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">回式年遷宮の諸祭・行事等の読み方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">世界文化遺産（製鉄・鉄鉱、造船、石炭産業）の読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">世界文化遺産・韮山反射炉関連の読み方　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4/22</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">言葉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">慣用的な読み方のあるＡＢＣ略語の意味・スペルも</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">外国語　字母表と読み方の原則（地名・人名）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">言葉・会社名など　にほん・にっぽん・５０音順で分類</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">過去のファイル（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2002</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2003</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">報道からの言葉を収集　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2019</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">年からは音訳の部屋リビングルーム参照</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">法人等略語の正式な法人名一覧表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東日本大震災・福島原発事故 報道からの言葉　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">御嶽山噴火 報道からの言葉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">平成２８年（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2016</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）熊本地震 報道からの言葉</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">オ・オン・ギョ・ゴ・ミ・その他　歴史用語　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">「大」「所」などの付く語　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">「油」「酢」「酒」「塩」の付く語</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">電話番号・郵便番号・住所・専門分野の数字など</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ISBN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">E-mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">・</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">の読み方</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">静岡県点字図書館</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">日本図書コード管理センター</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">報道等に使われる言葉をまとめる。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">図書や雑誌の関係用語・略語の情報　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ABC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">戦闘機・美容用語・ロケット・船・皇居関連用語・その他　</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2017</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">〜）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No.3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">N0.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">No.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（〜</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2009</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">自然</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">国土地理院等の読み方を参考に</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">音順に作成</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">活火山</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">（常時観測火山</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">47</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）の読み方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">84</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">主要活断層（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">98</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">断層帯）の読み方</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富士山に関する言葉。どうぞ言葉で登山を。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">一級河川の読み方　地域別５０音順　河川用語へリンク</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">主な湖沼の読み方　地域別</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">主な諸島・島の読み方　地域別</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地図・海図に記載する名称が決定した離島の読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岬の読み方 （崎・埼・碕・鼻）も含む</t>
+  </si>
+  <si>
+    <t xml:space="preserve">91</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">にほんの里</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">選</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">朝日新聞創刊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">130</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">周年記念事業</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">各種</t>
+  </si>
+  <si>
+    <t xml:space="preserve">出版社名の読み方　５０音順</t>
+  </si>
+  <si>
+    <t xml:space="preserve">93</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">雑誌・週刊誌の読み方　漢字と</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ABC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">順</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">行政地名以外</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">韓国・北朝鮮の地名・人名 読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">国立国語研究所による提案をまとめる。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">言葉の発音（文化庁による世論調査より）</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">読み方調査のための辞書・辞典・図鑑・専門書等</t>
+  </si>
+  <si>
+    <t xml:space="preserve">俳句作者の読み方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/haiku/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">参考</t>
+  </si>
+  <si>
+    <t xml:space="preserve">『第三版 俳句歳時記』（角川書店刊） 内山佐智子製作</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hiramatu-hifuka.com/onyak/image/momiji_r.gif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">国土地理院</t>
+  </si>
+  <si>
+    <t xml:space="preserve">地図記号一覧</t>
   </si>
 </sst>
 </file>
@@ -913,7 +2827,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Yu Gothic"/>
@@ -940,6 +2854,16 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -984,7 +2908,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -994,6 +2918,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2742,22 +4674,1964 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="97.39"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F106"/>
+  <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="90.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F78" s="4"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="F79" s="4"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F81" s="4"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="F82" s="4"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="F83" s="4"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F85" s="4"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="F86" s="4"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="F87" s="4"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F88" s="4"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F89" s="4"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F90" s="4"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F91" s="4"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F92" s="4"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F93" s="4"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="F94" s="4"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="F97" s="4"/>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F98" s="4"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="F99" s="4"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="F100" s="4"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F102" s="4"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="F103" s="4"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F104" s="4"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="4"/>
+      <c r="B105" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="4"/>
+      <c r="B106" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>201</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "NipponIkaJinmeiJiten" sheet in "OtoYakuNoHeyaYomikataJiten.xlsx" Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenNipponIkaJinmeiJitenMultimapFactoryBean.sheetName" property in "configuration.properties" Update "applicationContext.xml"
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="url_transition" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="link" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="TiZuKiGou" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="NipponIkaJinmeiJiten" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="852">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -3270,6 +3271,666 @@
   </si>
   <si>
     <t xml:space="preserve">うれつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安芸守貞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あきのもりさだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あきもりさだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浅井周伯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あざいしゅうはく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浅井貞庵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あざいていあん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浅井正封</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あざいまさよし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浅田宗伯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あさだそうはく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安倍真直</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あべのまなお</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有持桂里</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ありもちけいり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊沢蘭軒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いざわらんけん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石坂宗哲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いしざかそうてつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">出雲広貞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いずもひろさだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">井関玄悦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いぜきげんえつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">稲葉文礼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いなばぶんれい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">稲村三伯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いなむらさんぱく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">井上玄徹</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いのうえげんてつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇田川秦榛</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うだがわしんさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇津木昆台</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うつきこんだい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大槻玄沢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおつきげんたく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">緒方洪庵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おがたこうあん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岡本一抱</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おかもといっぽう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岡本玄冶</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おかもとげんや</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小川笙船</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おがわしょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">荻野元凱</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おぎのげんかい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奥劣斎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おくれっさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奥村良竹</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おくむらりょうちく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尾台榕堂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おだいようどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小野蘭山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おのらんざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">貝原益軒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かいばらえきけん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">賀川玄悦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かがわげんえつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">賀川玄迪</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かがわげんてき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香川修庵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かがわしゅうあん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香川修徳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かがわしゅうとく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">梶原性全</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かじわらせいぜん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">片倉鶴陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かたくらかくりょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桂川甫周</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かつらがわほしゅう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香月牛山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かつきぎゅうざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">加藤謙斎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かとうけんさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">亀井南冥</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かめいなんめい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北尾春圃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたおしゅんぼ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">喜多村直寛</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたむらちょっかん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北山友松</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたやまゆうしょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清川玄道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きよかわげんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小石玄俊</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こいしげんしゅん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後藤艮山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごとうごんざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごとうこんざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">坂浄運</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さかじょううん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">渋江抽斎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しぶえちゅうさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新宮涼庭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんぐうりょうてい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菅沼周桂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すがぬましゅうけい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菅原ミネ嗣</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すがわらのみねつぐ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">杉田玄白</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すぎたげんぱく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">杉山和一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すぎやまわいち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">多紀元胤</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たきげんいん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">多紀元簡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たきげんかん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">多紀元堅</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たきげんけん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">多紀元徳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たきげんとく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">竹田昌慶</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たけだしょうけい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田代三喜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たしろさんき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">丹波雅忠</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たんばまさただ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">丹波康頼</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たんばやすより</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津田玄仙</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つだげんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">戸田旭山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とだきょくざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">百百漢陰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">どどかんいん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">内藤希哲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ないとうきてつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中神琴渓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なかがみきんけい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中川修亭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なかがわしゅうてい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長沢道寿</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながさわどうじゅ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">永田徳本</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながたとくほん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">永富独嘯庵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながとみどくしょうあん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中西深斎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なかにししんさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中山三柳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なかやまさんりゅう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">半井明親</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なからいあきちか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">半井瑞策</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なからいずいさく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">半井卜養</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なからいぼくよう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">名古屋玄医</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なごやげんい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈須恒徳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なすこうとく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">野間玄琢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のまげんたく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">野呂元丈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のろげんじょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">華岡青洲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はなおかせいしゅう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">原南陽</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はらなんよう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深根輔仁</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふかねすけひと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福井楓亭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふくいふうてい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">古林見宜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふるばやしけんぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">堀正意</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほりせいい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本郷正豊</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほんごうせいほう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本間ソウ軒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほんまそうけん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松岡玄達</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつおかげんたつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松原慶輔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつばらけいすけ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">曲直瀬玄朔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まなせげんさく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">曲直瀬正純</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まなせしょうじゅん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">曲直瀬正淋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まなせしょうりん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">曲直瀬道三</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まなせどうさん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">御園意斎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みそのいさい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三輪東朔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みわとうさく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">村井琴山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むらいきんざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">目黒道琢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めぐろどうたく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">望月三英</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もちずきさんえい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">森立之</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もりりっし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">施薬院全宗</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やくいんぜんそう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山田業広</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまだぎょうこう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山田正珍</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまだせいちん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山脇東門</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまわきとうもん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山脇東洋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまわきとうよう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有隣</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆうりん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉雄耕牛</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よしおこうぎゅう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉田宗桂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よしだそうけい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉田宗恂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よしだそうじゅん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉益東洞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よしますとうどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉益南涯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よしますなんがい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">和気広世</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わけのひろよ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">和田東郭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わだとうかく</t>
   </si>
 </sst>
 </file>
@@ -3350,7 +4011,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3364,10 +4025,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3497,7 +4154,7 @@
   <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A1:B101"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5117,7 +5774,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="A1:B101"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5153,7 +5810,7 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="A1:B101 C23"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7094,822 +7751,1746 @@
   </sheetPr>
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>439</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>499</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>503</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="3" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>561</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="3" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="3" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="3" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="3" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="3" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="3" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="3" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="3" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="3" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="3" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="3" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="3" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="3" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="3" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="3" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="3" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="3" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="3" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="3" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="3" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4" t="s">
+      <c r="A91" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="3" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="4" t="s">
+      <c r="A92" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="3" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="4" t="s">
+      <c r="A94" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="3" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="3" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="3" t="s">
         <v>621</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="3" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="4" t="s">
+      <c r="A98" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>625</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="4" t="s">
+      <c r="A99" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="3" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="4" t="s">
+      <c r="A100" s="3" t="s">
         <v>628</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="3" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="4" t="s">
+      <c r="A101" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="3" t="s">
         <v>631</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B112"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.46"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>707</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>722</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>724</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="3" t="s">
+        <v>746</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="3" t="s">
+        <v>770</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="3" t="s">
+        <v>776</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="3" t="s">
+        <v>792</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="3" t="s">
+        <v>814</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="3" t="s">
+        <v>816</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="3" t="s">
+        <v>824</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="3" t="s">
+        <v>834</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="3" t="s">
+        <v>836</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="3" t="s">
+        <v>842</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="3" t="s">
+        <v>844</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="3" t="s">
+        <v>846</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "JRSenYomikataJiten" sheet in "OtoYakuNoHeyaYomikataJiten.xlsx" file Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenJRSenYomikataJitenMultimapFactoryBean.sheetName" property in "configuration.properties" Extends "org.springframework.beans.factory.StringMultiMapFromResourceFactoryBean" class by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenJRSenYomikataJitenMultimapFactoryBean" class Update "applicationContext.xml" Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenJRSenYomikataJitenMultimapFactoryBean.getObject()" method
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -16,6 +16,7 @@
     <sheet name="SansuuSuugakuYougoYomikataJiten" sheetId="6" state="visible" r:id="rId8"/>
     <sheet name="KisyoYougoYomikataJiten" sheetId="7" state="visible" r:id="rId9"/>
     <sheet name="RobottoYomikataJiten" sheetId="8" state="visible" r:id="rId10"/>
+    <sheet name="JRSenYomikataJiten" sheetId="9" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="6440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7350" uniqueCount="6796">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -20699,6 +20700,1074 @@
   <si>
     <t xml:space="preserve">たどころさとし</t>
   </si>
+  <si>
+    <t xml:space="preserve">江差線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えさしせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札沼線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっしょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石勝線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せきしょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石北線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せきほくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">釧網線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せんもうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宗谷線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">そうやせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千歳線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちとせせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津軽海峡線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つがるかいきょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">根室線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ねむろせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">函館線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はこだてせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日高線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひだかせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富良野線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふらのせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">室蘭線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むろらんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">留萌線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">るもいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吾妻線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あがつません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">赤羽線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あかばねせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">秋田新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あきたしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">左沢線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あてらざわせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">飯山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いいやません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石巻線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いしのまきせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">五日市線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いつかいちせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊東線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いとうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岩泉線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いわいずみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">羽越線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うえつせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">内房線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うちぼうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">越後線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えちごせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奥羽線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おううせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">青梅線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おうめせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大糸線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおいとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大船渡線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおふなとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大湊線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおみなとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">男鹿線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おがせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鹿島線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かしません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">釜石線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かまいしせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">烏山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">からすやません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">川越線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かわごえせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北上線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたかみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">久留里線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くるりせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">京浜東北線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">けいひんとうほくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">京葉線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">けいようせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">気仙沼線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">けせんぬません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小海線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">五能線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごのうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">埼京線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さいきょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">相模線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さがみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">井線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しののいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上越新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じょうえつしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上越線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じょうえつせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">常磐線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じょうばんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">信越線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんえつせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水郡線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すいぐんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仙山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せんざんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仙石線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せんせきせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">総武線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">そうぶせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">外房線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">そとぼうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高崎線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかさきせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田沢湖線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たざわこせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">只見線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ただみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中央線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちゅうおうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津軽線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つがるせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鶴見線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つるみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東海道線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうかいどうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東金線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうがねせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東北新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうほくしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東北線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうほくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長野新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながのしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">成田線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なりたせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">南武線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なんぶせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日光線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にっこうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">根岸線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ねぎしせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白新線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はくしんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">八高線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はちこうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">八戸線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はちのへせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">花輪線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はなわせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">磐越西線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばんえつさいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">磐越東線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばんえつとうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北陸新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほくりくしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水戸線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武蔵野線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むさしのせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">弥彦線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やひこせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山形新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまがたしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山田線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまだせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山手線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまのてせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">横須賀線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よこすかせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">横浜線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よこはません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">米坂線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よねさかせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陸羽西線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">りくうさいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陸羽東線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">りくうとうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">両毛線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">りょうもうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">飯田線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いいだせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">関西線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かんさいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">紀勢線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きせいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">御殿場線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごてんばせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">参宮線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんぐうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">太多線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たいたせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかやません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武豊線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たけとよせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東海道新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうかいどうしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">身延線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みのぶせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">名松線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めいしょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">赤穂線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あこうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">因美線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いんびせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇野線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うのせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇部線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うべせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">越美北線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えつみほくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">九頭竜線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くずりゅうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大阪環状線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおさかかんじょうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおさかひがしせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小野田線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おのだせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小浜線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おばません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">加古川線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かこがわせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">片町線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かたまちせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">可部線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かべせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">関西空港線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かんさいくうこうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岩徳線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">がんとくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">姫新線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きしんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">木次線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きすきせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉備線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きびせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">草津線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くさつせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">呉線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くれせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">芸備線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">げいびせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湖西線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こせいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">境線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さかいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桜井線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さくらいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桜島線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さくらじません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山陰線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんいんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三江線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんこうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山陽新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんようしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山陽線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんようせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">城端線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じょうはなせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新湊線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんみなとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瀬戸大橋線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せとおおはしせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つやません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富山港線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とやまこうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">七尾線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ななおせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈良線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ならせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">博多南線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はかたみなみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伯備線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はくびせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">播但線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばんたんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">阪和線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はんわせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">氷見線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福塩線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふくえんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福知山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふくちやません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北陸線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほくりくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本四備讃線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほんしびさんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">舞鶴線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まいづるせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">美祢線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みねせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山口線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまぐちせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">和歌山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わかやません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">内子線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うちこせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高徳線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうとくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">徳島線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とくしません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">土讃線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">どさんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鳴門線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なるとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">牟岐線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むぎせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">予讃線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よさんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">予土線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よどせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">指宿枕崎線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いぶすきまくらざきせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大村線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおむらせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鹿児島本</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かごしません</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香椎線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かしいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">唐津線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">からつせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">吉都線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きっとせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">九州新幹線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きゅうしゅうしんかんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">久大線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きゅうだいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後藤寺線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごとうじせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">篠栗線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ささぐりせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">佐世保線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">させぼせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">筑肥線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちくひせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">筑豊線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちくほうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長崎線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながさきせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日南線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にちなんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日豊線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にっぽうせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">肥薩線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひさつせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日田彦山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひたひこさんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">豊肥線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほうひせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三角線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みすみせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宮崎空港線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みやざきくうこうせん</t>
+  </si>
 </sst>
 </file>
 
@@ -20801,7 +21870,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -49080,14 +50149,14 @@
   </sheetPr>
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49102,7 +50171,7 @@
       <c r="A2" s="4" t="s">
         <v>6392</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6393</v>
       </c>
     </row>
@@ -49110,7 +50179,7 @@
       <c r="A3" s="4" t="s">
         <v>6394</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6395</v>
       </c>
     </row>
@@ -49118,7 +50187,7 @@
       <c r="A4" s="4" t="s">
         <v>6396</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6397</v>
       </c>
     </row>
@@ -49126,7 +50195,7 @@
       <c r="A5" s="4" t="s">
         <v>6398</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6399</v>
       </c>
     </row>
@@ -49134,7 +50203,7 @@
       <c r="A6" s="4" t="s">
         <v>6400</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>6401</v>
       </c>
     </row>
@@ -49142,7 +50211,7 @@
       <c r="A7" s="4" t="s">
         <v>6402</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>6403</v>
       </c>
     </row>
@@ -49150,7 +50219,7 @@
       <c r="A8" s="4" t="s">
         <v>6404</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>6405</v>
       </c>
     </row>
@@ -49158,7 +50227,7 @@
       <c r="A9" s="4" t="s">
         <v>6406</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>6407</v>
       </c>
     </row>
@@ -49166,7 +50235,7 @@
       <c r="A10" s="4" t="s">
         <v>6408</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>6409</v>
       </c>
     </row>
@@ -49174,7 +50243,7 @@
       <c r="A11" s="4" t="s">
         <v>6410</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>6411</v>
       </c>
     </row>
@@ -49182,7 +50251,7 @@
       <c r="A12" s="4" t="s">
         <v>6412</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>6413</v>
       </c>
     </row>
@@ -49190,7 +50259,7 @@
       <c r="A13" s="4" t="s">
         <v>6414</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>6415</v>
       </c>
     </row>
@@ -49198,7 +50267,7 @@
       <c r="A14" s="4" t="s">
         <v>6416</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>6417</v>
       </c>
     </row>
@@ -49206,7 +50275,7 @@
       <c r="A15" s="4" t="s">
         <v>6418</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>6419</v>
       </c>
     </row>
@@ -49214,7 +50283,7 @@
       <c r="A16" s="4" t="s">
         <v>6420</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>6421</v>
       </c>
     </row>
@@ -49222,7 +50291,7 @@
       <c r="A17" s="4" t="s">
         <v>6422</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>6423</v>
       </c>
     </row>
@@ -49230,7 +50299,7 @@
       <c r="A18" s="4" t="s">
         <v>6424</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>6425</v>
       </c>
     </row>
@@ -49238,7 +50307,7 @@
       <c r="A19" s="4" t="s">
         <v>6426</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>6427</v>
       </c>
     </row>
@@ -49246,7 +50315,7 @@
       <c r="A20" s="4" t="s">
         <v>6428</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>6429</v>
       </c>
     </row>
@@ -49254,7 +50323,7 @@
       <c r="A21" s="4" t="s">
         <v>6430</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>6431</v>
       </c>
     </row>
@@ -49262,7 +50331,7 @@
       <c r="A22" s="4" t="s">
         <v>6432</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>6433</v>
       </c>
     </row>
@@ -49270,7 +50339,7 @@
       <c r="A23" s="4" t="s">
         <v>6434</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>6435</v>
       </c>
     </row>
@@ -49278,7 +50347,7 @@
       <c r="A24" s="4" t="s">
         <v>6436</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>6437</v>
       </c>
     </row>
@@ -49286,8 +50355,1467 @@
       <c r="A25" s="4" t="s">
         <v>6438</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>6439</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B179"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>6440</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6441</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>6442</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6443</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6444</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6445</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6446</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>6447</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>6448</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6449</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6450</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6451</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>6452</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6453</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>6454</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6455</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>6456</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>6457</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>6458</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>6459</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>6460</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>6461</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>6462</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>6463</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>6464</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>6465</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>6466</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>6467</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>6468</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6469</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>6470</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>6471</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>6472</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>6473</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>6474</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>6475</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>6476</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>6477</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>6478</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>6479</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>6480</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>6481</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>6482</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>6483</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>6484</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>6485</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>6486</v>
+      </c>
       <c r="B25" s="0" t="s">
-        <v>6439</v>
+        <v>6487</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>6488</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>6489</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>6490</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>6491</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>6492</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>6493</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>6494</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>6495</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>6496</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>6497</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>6498</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>6499</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>6500</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>6501</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>6502</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>6503</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>6504</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>6505</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>6506</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>6507</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>6508</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>6509</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>6510</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>6511</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>6512</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>6513</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>6514</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>6515</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>6516</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>6517</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>6518</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>6519</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>6520</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>6521</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>6522</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>6523</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>6524</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>6525</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>6526</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>6527</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>6528</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>6529</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>6530</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>6531</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>6532</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>6533</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>6534</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>6535</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>6536</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>6537</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>6538</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>6539</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>6540</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>6541</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>6542</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>6543</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>6544</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>6545</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>6546</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>6547</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>6548</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>6549</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>6550</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>6551</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>6552</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>6553</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>6554</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>6555</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>6556</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>6557</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>6558</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>6559</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>6560</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>6561</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>6562</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>6563</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>6564</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>6565</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>6566</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>6567</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>6568</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>6569</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>6570</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>6571</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>6572</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>6573</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>6574</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>6575</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>6576</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>6577</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>6578</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>6579</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>6580</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>6581</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>6582</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>6583</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>6584</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>6585</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>6586</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>6587</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>6588</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>6589</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>6590</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>6591</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>6592</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>6593</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>6594</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>6595</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>6596</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>6597</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>6598</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>6599</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>6600</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>6601</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>6602</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>6603</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>6604</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>6605</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>6606</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>6607</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>6608</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>6609</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>6610</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>6611</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>6612</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>6613</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>6614</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>6615</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>6616</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>6617</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>6618</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>6619</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>6620</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>6621</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>6622</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>6623</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>6624</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>6625</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>6626</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>6627</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>6628</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>6629</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>6630</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>6631</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>6632</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>6633</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>6634</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>6635</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>6636</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>6637</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>6638</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>6639</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>6640</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>6641</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>6642</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>6643</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>6644</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>6645</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>6646</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>6647</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>6648</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>6649</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>6650</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>6651</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>6652</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>6653</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>6654</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>6655</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>6656</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>6657</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>6658</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>6659</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>6660</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>6661</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>6662</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>6663</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>6664</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>6665</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>6666</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>6667</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>6668</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>6669</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>6670</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>6671</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>6672</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>6673</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>6674</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>6675</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>6676</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>6677</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>6678</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>6679</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>6680</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>6681</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>6682</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>6683</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>6684</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>6685</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>6686</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>6688</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>6689</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>6690</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>6691</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>6692</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>6693</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>6694</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>6695</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>6696</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>6697</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>6698</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>6699</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>6700</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>6701</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>6702</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>6703</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>6704</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>6705</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>6706</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>6707</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>6708</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>6709</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>6710</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>6711</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>6712</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>6713</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>6714</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>6715</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>6716</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>6717</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>6718</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>6719</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>6720</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>6721</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>6722</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>6723</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>6724</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>6725</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>6726</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>6727</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>6728</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>6729</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>6730</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>6731</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>6732</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>6733</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>6734</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>6735</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>6736</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>6737</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>6738</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>6739</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>6740</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>6741</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>6742</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>6743</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>6744</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>6745</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>6746</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>6747</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>6748</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>6749</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>6750</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>6751</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>6752</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>6753</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>6754</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>6755</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>6756</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>6757</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>6758</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>6759</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>6760</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>6761</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>6762</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>6763</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>6764</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>6765</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>6766</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>6767</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>6768</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>6769</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>6770</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>6771</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>6772</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>6773</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>6774</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>6775</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>6776</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>6777</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>6778</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>6779</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>6780</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>6781</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>6782</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>6783</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>6784</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>6785</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>6786</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>6787</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>6788</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>6789</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>6790</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>6791</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>6792</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>6793</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>6794</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>6795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "SintomeiYomikataJiten" sheet in "OtoYakuNoHeyaYomikataJiten.xlsx" file Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenSintomeiYomikataJitenMultimapFactoryBean.sheetName" property in "configuration.properties" Extends "org.springframework.beans.factory.StringMultiMapFromResourceFactoryBean" class by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenSintomeiYomikataJitenMultimapFactoryBean" Class Update "applicationContext.xml" Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenSintomeiYomikataJitenMultimapFactoryBean.getObject()" method
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -18,6 +18,7 @@
     <sheet name="RobottoYomikataJiten" sheetId="8" state="visible" r:id="rId10"/>
     <sheet name="JRSenYomikataJiten" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="MintetsuYomikataJiten" sheetId="10" state="visible" r:id="rId12"/>
+    <sheet name="SintomeiYomikataJiten" sheetId="11" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8426" uniqueCount="7854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8502" uniqueCount="7928">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -24942,6 +24943,228 @@
   </si>
   <si>
     <t xml:space="preserve">くろべきょうこくてつどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">御殿場</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごてんば</t>
+  </si>
+  <si>
+    <t xml:space="preserve">御殿場市駒門</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごてんばしこまかど</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長泉沼津</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながいずみぬまづ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">駿東郡長泉町元長窪</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すんとうぐんながいずみちょうもとながくぼ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">駿河湾沼津</t>
+  </si>
+  <si>
+    <t xml:space="preserve">するがわんぬまづ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">沼津市根古屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ぬまづしねごや</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新富士</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんふじ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富士市厚原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじしあつはら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新清水</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんしみず</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市清水区宍原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかししみずくししはら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清水</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しみず</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市清水区小河内</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかししみずくこごうち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市清水区吉原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかししみずくよしわら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市清水区杉山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかししみずくすぎやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新静岡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんしずおか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市葵区下</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかしあおいくしも</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市葵区小瀬戸</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかしあおいくこぜと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静岡市葵区飯間</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずおかしあおいくはんま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">藤枝岡部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじえだおかべ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">藤枝市岡部町入野</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじえだしおかべちょういりの</t>
+  </si>
+  <si>
+    <t xml:space="preserve">藤枝</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじえだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">藤枝市花倉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじえだしはなぐら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">島田金谷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しまだかなや</t>
+  </si>
+  <si>
+    <t xml:space="preserve">島田市横岡新田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しまだしよこおかしんでん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">掛川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かけがわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">掛川市倉真</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かけがわしくらみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">森掛川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もりかけがわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">周智郡森町睦実</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しゅうちぐんもりまちむつみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">遠州森町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えんしゅうもりまち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">周智郡森町円田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しゅうちぐんもりまちえんでん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜松浜北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はままつはまきた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜松市浜北区中瀬</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はままつしはまきたくなかぜ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜松</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はままつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜松市浜北区四大地</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はままつしはまきたくよんだいち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜松市北区引佐町東黒田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はままつしきたくいなさちょうひがしくろだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新東名高速道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんとうめいこうそくどうろ</t>
   </si>
 </sst>
 </file>
@@ -26794,13 +27017,13 @@
   </sheetPr>
   <dimension ref="A1:B538"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="39.55"/>
   </cols>
   <sheetData>
@@ -28237,7 +28460,7 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
+      <c r="A180" s="1" t="s">
         <v>7145</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -28245,7 +28468,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
+      <c r="A181" s="1" t="s">
         <v>7147</v>
       </c>
       <c r="B181" s="1" t="s">
@@ -28253,7 +28476,7 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
+      <c r="A182" s="1" t="s">
         <v>7149</v>
       </c>
       <c r="B182" s="1" t="s">
@@ -28261,7 +28484,7 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
+      <c r="A183" s="1" t="s">
         <v>7151</v>
       </c>
       <c r="B183" s="1" t="s">
@@ -28269,7 +28492,7 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
+      <c r="A184" s="1" t="s">
         <v>7153</v>
       </c>
       <c r="B184" s="1" t="s">
@@ -28277,7 +28500,7 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
+      <c r="A185" s="1" t="s">
         <v>7155</v>
       </c>
       <c r="B185" s="1" t="s">
@@ -28285,7 +28508,7 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
+      <c r="A186" s="1" t="s">
         <v>7157</v>
       </c>
       <c r="B186" s="1" t="s">
@@ -28293,7 +28516,7 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
+      <c r="A187" s="1" t="s">
         <v>7159</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -28301,7 +28524,7 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
+      <c r="A188" s="1" t="s">
         <v>7161</v>
       </c>
       <c r="B188" s="1" t="s">
@@ -28309,7 +28532,7 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
+      <c r="A189" s="1" t="s">
         <v>7163</v>
       </c>
       <c r="B189" s="1" t="s">
@@ -28317,7 +28540,7 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
+      <c r="A190" s="1" t="s">
         <v>7165</v>
       </c>
       <c r="B190" s="1" t="s">
@@ -28325,7 +28548,7 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
+      <c r="A191" s="1" t="s">
         <v>7167</v>
       </c>
       <c r="B191" s="1" t="s">
@@ -28333,7 +28556,7 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
+      <c r="A192" s="1" t="s">
         <v>7169</v>
       </c>
       <c r="B192" s="1" t="s">
@@ -28341,7 +28564,7 @@
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
+      <c r="A193" s="1" t="s">
         <v>7171</v>
       </c>
       <c r="B193" s="1" t="s">
@@ -28349,7 +28572,7 @@
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
+      <c r="A194" s="1" t="s">
         <v>7173</v>
       </c>
       <c r="B194" s="1" t="s">
@@ -28357,7 +28580,7 @@
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
+      <c r="A195" s="1" t="s">
         <v>7175</v>
       </c>
       <c r="B195" s="1" t="s">
@@ -28365,7 +28588,7 @@
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
+      <c r="A196" s="1" t="s">
         <v>7177</v>
       </c>
       <c r="B196" s="1" t="s">
@@ -28373,7 +28596,7 @@
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
+      <c r="A197" s="1" t="s">
         <v>7179</v>
       </c>
       <c r="B197" s="1" t="s">
@@ -28381,7 +28604,7 @@
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
+      <c r="A198" s="1" t="s">
         <v>7181</v>
       </c>
       <c r="B198" s="1" t="s">
@@ -28389,7 +28612,7 @@
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
+      <c r="A199" s="1" t="s">
         <v>7183</v>
       </c>
       <c r="B199" s="1" t="s">
@@ -28397,7 +28620,7 @@
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
+      <c r="A200" s="1" t="s">
         <v>7185</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -28405,7 +28628,7 @@
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
+      <c r="A201" s="1" t="s">
         <v>7187</v>
       </c>
       <c r="B201" s="1" t="s">
@@ -28413,7 +28636,7 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
+      <c r="A202" s="1" t="s">
         <v>7189</v>
       </c>
       <c r="B202" s="1" t="s">
@@ -28421,7 +28644,7 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
+      <c r="A203" s="1" t="s">
         <v>7191</v>
       </c>
       <c r="B203" s="1" t="s">
@@ -28429,7 +28652,7 @@
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
+      <c r="A204" s="1" t="s">
         <v>7193</v>
       </c>
       <c r="B204" s="1" t="s">
@@ -28437,7 +28660,7 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
+      <c r="A205" s="1" t="s">
         <v>7195</v>
       </c>
       <c r="B205" s="1" t="s">
@@ -28445,7 +28668,7 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="0" t="s">
+      <c r="A206" s="1" t="s">
         <v>7197</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -28453,7 +28676,7 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="s">
+      <c r="A207" s="1" t="s">
         <v>7199</v>
       </c>
       <c r="B207" s="1" t="s">
@@ -28461,7 +28684,7 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
+      <c r="A208" s="1" t="s">
         <v>7201</v>
       </c>
       <c r="B208" s="1" t="s">
@@ -28469,7 +28692,7 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="0" t="s">
+      <c r="A209" s="1" t="s">
         <v>6734</v>
       </c>
       <c r="B209" s="1" t="s">
@@ -28477,7 +28700,7 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
+      <c r="A210" s="1" t="s">
         <v>7203</v>
       </c>
       <c r="B210" s="1" t="s">
@@ -28485,7 +28708,7 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
+      <c r="A211" s="1" t="s">
         <v>6602</v>
       </c>
       <c r="B211" s="1" t="s">
@@ -28493,7 +28716,7 @@
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="0" t="s">
+      <c r="A212" s="1" t="s">
         <v>7205</v>
       </c>
       <c r="B212" s="1" t="s">
@@ -28501,7 +28724,7 @@
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="0" t="s">
+      <c r="A213" s="1" t="s">
         <v>7207</v>
       </c>
       <c r="B213" s="1" t="s">
@@ -28509,7 +28732,7 @@
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="0" t="s">
+      <c r="A214" s="1" t="s">
         <v>7209</v>
       </c>
       <c r="B214" s="1" t="s">
@@ -28517,7 +28740,7 @@
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
+      <c r="A215" s="1" t="s">
         <v>7211</v>
       </c>
       <c r="B215" s="1" t="s">
@@ -28525,7 +28748,7 @@
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
+      <c r="A216" s="1" t="s">
         <v>7213</v>
       </c>
       <c r="B216" s="1" t="s">
@@ -28533,7 +28756,7 @@
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
+      <c r="A217" s="1" t="s">
         <v>7215</v>
       </c>
       <c r="B217" s="1" t="s">
@@ -28541,7 +28764,7 @@
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="0" t="s">
+      <c r="A218" s="1" t="s">
         <v>7217</v>
       </c>
       <c r="B218" s="1" t="s">
@@ -28549,7 +28772,7 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
+      <c r="A219" s="1" t="s">
         <v>7219</v>
       </c>
       <c r="B219" s="1" t="s">
@@ -28557,7 +28780,7 @@
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="0" t="s">
+      <c r="A220" s="1" t="s">
         <v>7221</v>
       </c>
       <c r="B220" s="1" t="s">
@@ -28565,7 +28788,7 @@
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A221" s="0" t="s">
+      <c r="A221" s="1" t="s">
         <v>7223</v>
       </c>
       <c r="B221" s="1" t="s">
@@ -28573,7 +28796,7 @@
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="0" t="s">
+      <c r="A222" s="1" t="s">
         <v>7225</v>
       </c>
       <c r="B222" s="1" t="s">
@@ -28581,7 +28804,7 @@
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="0" t="s">
+      <c r="A223" s="1" t="s">
         <v>7227</v>
       </c>
       <c r="B223" s="1" t="s">
@@ -28589,7 +28812,7 @@
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
+      <c r="A224" s="1" t="s">
         <v>7229</v>
       </c>
       <c r="B224" s="1" t="s">
@@ -28597,7 +28820,7 @@
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="0" t="s">
+      <c r="A225" s="1" t="s">
         <v>7231</v>
       </c>
       <c r="B225" s="1" t="s">
@@ -28605,7 +28828,7 @@
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="0" t="s">
+      <c r="A226" s="1" t="s">
         <v>7233</v>
       </c>
       <c r="B226" s="1" t="s">
@@ -28613,7 +28836,7 @@
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="0" t="s">
+      <c r="A227" s="1" t="s">
         <v>7235</v>
       </c>
       <c r="B227" s="1" t="s">
@@ -28621,7 +28844,7 @@
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="0" t="s">
+      <c r="A228" s="1" t="s">
         <v>7237</v>
       </c>
       <c r="B228" s="1" t="s">
@@ -28629,7 +28852,7 @@
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="0" t="s">
+      <c r="A229" s="1" t="s">
         <v>7239</v>
       </c>
       <c r="B229" s="1" t="s">
@@ -28637,7 +28860,7 @@
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="0" t="s">
+      <c r="A230" s="1" t="s">
         <v>7241</v>
       </c>
       <c r="B230" s="1" t="s">
@@ -28645,7 +28868,7 @@
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="0" t="s">
+      <c r="A231" s="1" t="s">
         <v>7243</v>
       </c>
       <c r="B231" s="1" t="s">
@@ -28653,7 +28876,7 @@
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="0" t="s">
+      <c r="A232" s="1" t="s">
         <v>7245</v>
       </c>
       <c r="B232" s="1" t="s">
@@ -28661,7 +28884,7 @@
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="0" t="s">
+      <c r="A233" s="1" t="s">
         <v>7247</v>
       </c>
       <c r="B233" s="1" t="s">
@@ -28669,7 +28892,7 @@
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="0" t="s">
+      <c r="A234" s="1" t="s">
         <v>7249</v>
       </c>
       <c r="B234" s="1" t="s">
@@ -28677,7 +28900,7 @@
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="0" t="s">
+      <c r="A235" s="1" t="s">
         <v>7251</v>
       </c>
       <c r="B235" s="1" t="s">
@@ -28685,7 +28908,7 @@
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="0" t="s">
+      <c r="A236" s="1" t="s">
         <v>7253</v>
       </c>
       <c r="B236" s="1" t="s">
@@ -28693,7 +28916,7 @@
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="0" t="s">
+      <c r="A237" s="1" t="s">
         <v>7255</v>
       </c>
       <c r="B237" s="1" t="s">
@@ -28701,7 +28924,7 @@
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="0" t="s">
+      <c r="A238" s="1" t="s">
         <v>7257</v>
       </c>
       <c r="B238" s="1" t="s">
@@ -28709,7 +28932,7 @@
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="0" t="s">
+      <c r="A239" s="1" t="s">
         <v>7259</v>
       </c>
       <c r="B239" s="1" t="s">
@@ -28717,7 +28940,7 @@
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="0" t="s">
+      <c r="A240" s="1" t="s">
         <v>7261</v>
       </c>
       <c r="B240" s="1" t="s">
@@ -28725,7 +28948,7 @@
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="0" t="s">
+      <c r="A241" s="1" t="s">
         <v>7263</v>
       </c>
       <c r="B241" s="1" t="s">
@@ -28733,7 +28956,7 @@
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="0" t="s">
+      <c r="A242" s="1" t="s">
         <v>7265</v>
       </c>
       <c r="B242" s="1" t="s">
@@ -28741,7 +28964,7 @@
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="0" t="s">
+      <c r="A243" s="1" t="s">
         <v>7267</v>
       </c>
       <c r="B243" s="1" t="s">
@@ -28749,7 +28972,7 @@
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="0" t="s">
+      <c r="A244" s="1" t="s">
         <v>7269</v>
       </c>
       <c r="B244" s="1" t="s">
@@ -28757,7 +28980,7 @@
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="0" t="s">
+      <c r="A245" s="1" t="s">
         <v>7271</v>
       </c>
       <c r="B245" s="1" t="s">
@@ -28765,7 +28988,7 @@
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="0" t="s">
+      <c r="A246" s="1" t="s">
         <v>7273</v>
       </c>
       <c r="B246" s="1" t="s">
@@ -28773,7 +28996,7 @@
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="0" t="s">
+      <c r="A247" s="1" t="s">
         <v>7275</v>
       </c>
       <c r="B247" s="1" t="s">
@@ -28781,7 +29004,7 @@
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="0" t="s">
+      <c r="A248" s="1" t="s">
         <v>7277</v>
       </c>
       <c r="B248" s="1" t="s">
@@ -28789,7 +29012,7 @@
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="0" t="s">
+      <c r="A249" s="1" t="s">
         <v>7279</v>
       </c>
       <c r="B249" s="1" t="s">
@@ -28797,7 +29020,7 @@
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="0" t="s">
+      <c r="A250" s="1" t="s">
         <v>7281</v>
       </c>
       <c r="B250" s="1" t="s">
@@ -28805,7 +29028,7 @@
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="0" t="s">
+      <c r="A251" s="1" t="s">
         <v>7283</v>
       </c>
       <c r="B251" s="1" t="s">
@@ -28813,7 +29036,7 @@
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="0" t="s">
+      <c r="A252" s="1" t="s">
         <v>7285</v>
       </c>
       <c r="B252" s="1" t="s">
@@ -28821,7 +29044,7 @@
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="0" t="s">
+      <c r="A253" s="1" t="s">
         <v>7287</v>
       </c>
       <c r="B253" s="1" t="s">
@@ -28829,7 +29052,7 @@
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="0" t="s">
+      <c r="A254" s="1" t="s">
         <v>7289</v>
       </c>
       <c r="B254" s="1" t="s">
@@ -28837,7 +29060,7 @@
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="0" t="s">
+      <c r="A255" s="1" t="s">
         <v>7291</v>
       </c>
       <c r="B255" s="1" t="s">
@@ -28845,7 +29068,7 @@
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="0" t="s">
+      <c r="A256" s="1" t="s">
         <v>7293</v>
       </c>
       <c r="B256" s="1" t="s">
@@ -28853,7 +29076,7 @@
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="0" t="s">
+      <c r="A257" s="1" t="s">
         <v>7295</v>
       </c>
       <c r="B257" s="1" t="s">
@@ -28861,7 +29084,7 @@
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="0" t="s">
+      <c r="A258" s="1" t="s">
         <v>7297</v>
       </c>
       <c r="B258" s="1" t="s">
@@ -28869,7 +29092,7 @@
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="0" t="s">
+      <c r="A259" s="1" t="s">
         <v>6576</v>
       </c>
       <c r="B259" s="1" t="s">
@@ -28877,7 +29100,7 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="0" t="s">
+      <c r="A260" s="1" t="s">
         <v>7299</v>
       </c>
       <c r="B260" s="1" t="s">
@@ -28885,7 +29108,7 @@
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="0" t="s">
+      <c r="A261" s="1" t="s">
         <v>7301</v>
       </c>
       <c r="B261" s="1" t="s">
@@ -28893,7 +29116,7 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="0" t="s">
+      <c r="A262" s="1" t="s">
         <v>7303</v>
       </c>
       <c r="B262" s="1" t="s">
@@ -28901,7 +29124,7 @@
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="0" t="s">
+      <c r="A263" s="1" t="s">
         <v>7305</v>
       </c>
       <c r="B263" s="1" t="s">
@@ -28909,7 +29132,7 @@
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="0" t="s">
+      <c r="A264" s="1" t="s">
         <v>7307</v>
       </c>
       <c r="B264" s="1" t="s">
@@ -28917,7 +29140,7 @@
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="0" t="s">
+      <c r="A265" s="1" t="s">
         <v>7309</v>
       </c>
       <c r="B265" s="1" t="s">
@@ -28925,7 +29148,7 @@
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="0" t="s">
+      <c r="A266" s="1" t="s">
         <v>7311</v>
       </c>
       <c r="B266" s="1" t="s">
@@ -28933,7 +29156,7 @@
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="0" t="s">
+      <c r="A267" s="1" t="s">
         <v>7313</v>
       </c>
       <c r="B267" s="1" t="s">
@@ -28941,7 +29164,7 @@
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="0" t="s">
+      <c r="A268" s="1" t="s">
         <v>7315</v>
       </c>
       <c r="B268" s="1" t="s">
@@ -28949,7 +29172,7 @@
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="0" t="s">
+      <c r="A269" s="1" t="s">
         <v>7317</v>
       </c>
       <c r="B269" s="1" t="s">
@@ -28957,7 +29180,7 @@
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="0" t="s">
+      <c r="A270" s="1" t="s">
         <v>7319</v>
       </c>
       <c r="B270" s="1" t="s">
@@ -28965,7 +29188,7 @@
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="0" t="s">
+      <c r="A271" s="1" t="s">
         <v>7321</v>
       </c>
       <c r="B271" s="1" t="s">
@@ -28973,7 +29196,7 @@
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="0" t="s">
+      <c r="A272" s="1" t="s">
         <v>7323</v>
       </c>
       <c r="B272" s="1" t="s">
@@ -28981,7 +29204,7 @@
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="0" t="s">
+      <c r="A273" s="1" t="s">
         <v>7325</v>
       </c>
       <c r="B273" s="1" t="s">
@@ -28989,7 +29212,7 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="0" t="s">
+      <c r="A274" s="1" t="s">
         <v>7327</v>
       </c>
       <c r="B274" s="1" t="s">
@@ -28997,7 +29220,7 @@
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="0" t="s">
+      <c r="A275" s="1" t="s">
         <v>7329</v>
       </c>
       <c r="B275" s="1" t="s">
@@ -29005,7 +29228,7 @@
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="0" t="s">
+      <c r="A276" s="1" t="s">
         <v>7331</v>
       </c>
       <c r="B276" s="1" t="s">
@@ -29013,7 +29236,7 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="0" t="s">
+      <c r="A277" s="1" t="s">
         <v>7333</v>
       </c>
       <c r="B277" s="1" t="s">
@@ -29021,7 +29244,7 @@
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="0" t="s">
+      <c r="A278" s="1" t="s">
         <v>7335</v>
       </c>
       <c r="B278" s="1" t="s">
@@ -29029,7 +29252,7 @@
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="0" t="s">
+      <c r="A279" s="1" t="s">
         <v>7337</v>
       </c>
       <c r="B279" s="1" t="s">
@@ -29037,7 +29260,7 @@
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="0" t="s">
+      <c r="A280" s="1" t="s">
         <v>7339</v>
       </c>
       <c r="B280" s="1" t="s">
@@ -29045,7 +29268,7 @@
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="0" t="s">
+      <c r="A281" s="1" t="s">
         <v>7341</v>
       </c>
       <c r="B281" s="1" t="s">
@@ -29053,7 +29276,7 @@
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="0" t="s">
+      <c r="A282" s="1" t="s">
         <v>7343</v>
       </c>
       <c r="B282" s="1" t="s">
@@ -29061,7 +29284,7 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="0" t="s">
+      <c r="A283" s="1" t="s">
         <v>7345</v>
       </c>
       <c r="B283" s="1" t="s">
@@ -29069,7 +29292,7 @@
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="0" t="s">
+      <c r="A284" s="1" t="s">
         <v>7347</v>
       </c>
       <c r="B284" s="1" t="s">
@@ -29077,7 +29300,7 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="0" t="s">
+      <c r="A285" s="1" t="s">
         <v>7349</v>
       </c>
       <c r="B285" s="1" t="s">
@@ -29085,7 +29308,7 @@
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="0" t="s">
+      <c r="A286" s="1" t="s">
         <v>7351</v>
       </c>
       <c r="B286" s="1" t="s">
@@ -29093,7 +29316,7 @@
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="0" t="s">
+      <c r="A287" s="1" t="s">
         <v>7353</v>
       </c>
       <c r="B287" s="1" t="s">
@@ -29101,7 +29324,7 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="0" t="s">
+      <c r="A288" s="1" t="s">
         <v>7355</v>
       </c>
       <c r="B288" s="1" t="s">
@@ -29109,7 +29332,7 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="0" t="s">
+      <c r="A289" s="1" t="s">
         <v>7357</v>
       </c>
       <c r="B289" s="1" t="s">
@@ -29117,7 +29340,7 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="0" t="s">
+      <c r="A290" s="1" t="s">
         <v>7359</v>
       </c>
       <c r="B290" s="1" t="s">
@@ -29125,7 +29348,7 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="0" t="s">
+      <c r="A291" s="1" t="s">
         <v>7361</v>
       </c>
       <c r="B291" s="1" t="s">
@@ -29133,7 +29356,7 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="0" t="s">
+      <c r="A292" s="1" t="s">
         <v>7363</v>
       </c>
       <c r="B292" s="1" t="s">
@@ -29141,7 +29364,7 @@
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="0" t="s">
+      <c r="A293" s="1" t="s">
         <v>7364</v>
       </c>
       <c r="B293" s="1" t="s">
@@ -29149,7 +29372,7 @@
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="0" t="s">
+      <c r="A294" s="1" t="s">
         <v>7366</v>
       </c>
       <c r="B294" s="1" t="s">
@@ -29157,7 +29380,7 @@
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="0" t="s">
+      <c r="A295" s="1" t="s">
         <v>7368</v>
       </c>
       <c r="B295" s="1" t="s">
@@ -29165,7 +29388,7 @@
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="0" t="s">
+      <c r="A296" s="1" t="s">
         <v>7370</v>
       </c>
       <c r="B296" s="1" t="s">
@@ -29173,7 +29396,7 @@
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="0" t="s">
+      <c r="A297" s="1" t="s">
         <v>7372</v>
       </c>
       <c r="B297" s="1" t="s">
@@ -29181,7 +29404,7 @@
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="0" t="s">
+      <c r="A298" s="1" t="s">
         <v>7374</v>
       </c>
       <c r="B298" s="1" t="s">
@@ -29189,7 +29412,7 @@
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="0" t="s">
+      <c r="A299" s="1" t="s">
         <v>7376</v>
       </c>
       <c r="B299" s="1" t="s">
@@ -29197,7 +29420,7 @@
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="0" t="s">
+      <c r="A300" s="1" t="s">
         <v>7378</v>
       </c>
       <c r="B300" s="1" t="s">
@@ -29205,7 +29428,7 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="0" t="s">
+      <c r="A301" s="1" t="s">
         <v>7380</v>
       </c>
       <c r="B301" s="1" t="s">
@@ -29213,7 +29436,7 @@
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="0" t="s">
+      <c r="A302" s="1" t="s">
         <v>7382</v>
       </c>
       <c r="B302" s="1" t="s">
@@ -29221,7 +29444,7 @@
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="0" t="s">
+      <c r="A303" s="1" t="s">
         <v>7384</v>
       </c>
       <c r="B303" s="1" t="s">
@@ -29229,7 +29452,7 @@
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="0" t="s">
+      <c r="A304" s="1" t="s">
         <v>7386</v>
       </c>
       <c r="B304" s="1" t="s">
@@ -29237,7 +29460,7 @@
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="0" t="s">
+      <c r="A305" s="1" t="s">
         <v>7388</v>
       </c>
       <c r="B305" s="1" t="s">
@@ -29245,7 +29468,7 @@
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="0" t="s">
+      <c r="A306" s="1" t="s">
         <v>7390</v>
       </c>
       <c r="B306" s="1" t="s">
@@ -29253,7 +29476,7 @@
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A307" s="0" t="s">
+      <c r="A307" s="1" t="s">
         <v>7392</v>
       </c>
       <c r="B307" s="1" t="s">
@@ -29261,7 +29484,7 @@
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="0" t="s">
+      <c r="A308" s="1" t="s">
         <v>7394</v>
       </c>
       <c r="B308" s="1" t="s">
@@ -29269,7 +29492,7 @@
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="0" t="s">
+      <c r="A309" s="1" t="s">
         <v>7396</v>
       </c>
       <c r="B309" s="1" t="s">
@@ -29277,7 +29500,7 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="0" t="s">
+      <c r="A310" s="1" t="s">
         <v>7398</v>
       </c>
       <c r="B310" s="1" t="s">
@@ -29285,7 +29508,7 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="0" t="s">
+      <c r="A311" s="1" t="s">
         <v>7400</v>
       </c>
       <c r="B311" s="1" t="s">
@@ -29293,7 +29516,7 @@
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="0" t="s">
+      <c r="A312" s="1" t="s">
         <v>7402</v>
       </c>
       <c r="B312" s="1" t="s">
@@ -29301,7 +29524,7 @@
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="0" t="s">
+      <c r="A313" s="1" t="s">
         <v>7404</v>
       </c>
       <c r="B313" s="1" t="s">
@@ -29309,7 +29532,7 @@
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="0" t="s">
+      <c r="A314" s="1" t="s">
         <v>7406</v>
       </c>
       <c r="B314" s="1" t="s">
@@ -29317,7 +29540,7 @@
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="0" t="s">
+      <c r="A315" s="1" t="s">
         <v>7408</v>
       </c>
       <c r="B315" s="1" t="s">
@@ -29325,7 +29548,7 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="0" t="s">
+      <c r="A316" s="1" t="s">
         <v>7410</v>
       </c>
       <c r="B316" s="1" t="s">
@@ -29333,7 +29556,7 @@
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="0" t="s">
+      <c r="A317" s="1" t="s">
         <v>7412</v>
       </c>
       <c r="B317" s="1" t="s">
@@ -29341,7 +29564,7 @@
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="0" t="s">
+      <c r="A318" s="1" t="s">
         <v>7414</v>
       </c>
       <c r="B318" s="1" t="s">
@@ -29349,7 +29572,7 @@
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="0" t="s">
+      <c r="A319" s="1" t="s">
         <v>7416</v>
       </c>
       <c r="B319" s="1" t="s">
@@ -29357,7 +29580,7 @@
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="0" t="s">
+      <c r="A320" s="1" t="s">
         <v>7418</v>
       </c>
       <c r="B320" s="1" t="s">
@@ -29365,7 +29588,7 @@
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="0" t="s">
+      <c r="A321" s="1" t="s">
         <v>7420</v>
       </c>
       <c r="B321" s="1" t="s">
@@ -29373,7 +29596,7 @@
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="0" t="s">
+      <c r="A322" s="1" t="s">
         <v>7422</v>
       </c>
       <c r="B322" s="1" t="s">
@@ -29381,7 +29604,7 @@
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A323" s="0" t="s">
+      <c r="A323" s="1" t="s">
         <v>7424</v>
       </c>
       <c r="B323" s="1" t="s">
@@ -29389,7 +29612,7 @@
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="0" t="s">
+      <c r="A324" s="1" t="s">
         <v>7426</v>
       </c>
       <c r="B324" s="1" t="s">
@@ -29397,7 +29620,7 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="0" t="s">
+      <c r="A325" s="1" t="s">
         <v>7428</v>
       </c>
       <c r="B325" s="1" t="s">
@@ -29405,7 +29628,7 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="0" t="s">
+      <c r="A326" s="1" t="s">
         <v>7430</v>
       </c>
       <c r="B326" s="1" t="s">
@@ -29413,7 +29636,7 @@
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="0" t="s">
+      <c r="A327" s="1" t="s">
         <v>7432</v>
       </c>
       <c r="B327" s="1" t="s">
@@ -29421,7 +29644,7 @@
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="0" t="s">
+      <c r="A328" s="1" t="s">
         <v>7434</v>
       </c>
       <c r="B328" s="1" t="s">
@@ -29429,7 +29652,7 @@
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="0" t="s">
+      <c r="A329" s="1" t="s">
         <v>7436</v>
       </c>
       <c r="B329" s="1" t="s">
@@ -29437,7 +29660,7 @@
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="0" t="s">
+      <c r="A330" s="1" t="s">
         <v>7438</v>
       </c>
       <c r="B330" s="1" t="s">
@@ -29445,7 +29668,7 @@
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="0" t="s">
+      <c r="A331" s="1" t="s">
         <v>7440</v>
       </c>
       <c r="B331" s="1" t="s">
@@ -29453,7 +29676,7 @@
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="0" t="s">
+      <c r="A332" s="1" t="s">
         <v>7442</v>
       </c>
       <c r="B332" s="1" t="s">
@@ -29461,7 +29684,7 @@
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="0" t="s">
+      <c r="A333" s="1" t="s">
         <v>7444</v>
       </c>
       <c r="B333" s="1" t="s">
@@ -29469,7 +29692,7 @@
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A334" s="0" t="s">
+      <c r="A334" s="1" t="s">
         <v>7446</v>
       </c>
       <c r="B334" s="1" t="s">
@@ -29477,7 +29700,7 @@
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="0" t="s">
+      <c r="A335" s="1" t="s">
         <v>7448</v>
       </c>
       <c r="B335" s="1" t="s">
@@ -29485,7 +29708,7 @@
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="0" t="s">
+      <c r="A336" s="1" t="s">
         <v>7450</v>
       </c>
       <c r="B336" s="1" t="s">
@@ -29493,7 +29716,7 @@
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="0" t="s">
+      <c r="A337" s="1" t="s">
         <v>7452</v>
       </c>
       <c r="B337" s="1" t="s">
@@ -29501,7 +29724,7 @@
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="0" t="s">
+      <c r="A338" s="1" t="s">
         <v>7454</v>
       </c>
       <c r="B338" s="1" t="s">
@@ -29509,7 +29732,7 @@
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="0" t="s">
+      <c r="A339" s="1" t="s">
         <v>7456</v>
       </c>
       <c r="B339" s="1" t="s">
@@ -29517,7 +29740,7 @@
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="0" t="s">
+      <c r="A340" s="1" t="s">
         <v>7458</v>
       </c>
       <c r="B340" s="1" t="s">
@@ -29525,7 +29748,7 @@
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A341" s="0" t="s">
+      <c r="A341" s="1" t="s">
         <v>7460</v>
       </c>
       <c r="B341" s="1" t="s">
@@ -29533,7 +29756,7 @@
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A342" s="0" t="s">
+      <c r="A342" s="1" t="s">
         <v>7462</v>
       </c>
       <c r="B342" s="1" t="s">
@@ -29541,7 +29764,7 @@
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A343" s="0" t="s">
+      <c r="A343" s="1" t="s">
         <v>7464</v>
       </c>
       <c r="B343" s="1" t="s">
@@ -29549,7 +29772,7 @@
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A344" s="0" t="s">
+      <c r="A344" s="1" t="s">
         <v>7466</v>
       </c>
       <c r="B344" s="1" t="s">
@@ -29557,7 +29780,7 @@
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A345" s="0" t="s">
+      <c r="A345" s="1" t="s">
         <v>7468</v>
       </c>
       <c r="B345" s="1" t="s">
@@ -29565,7 +29788,7 @@
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A346" s="0" t="s">
+      <c r="A346" s="1" t="s">
         <v>7470</v>
       </c>
       <c r="B346" s="1" t="s">
@@ -29573,7 +29796,7 @@
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="0" t="s">
+      <c r="A347" s="1" t="s">
         <v>7472</v>
       </c>
       <c r="B347" s="1" t="s">
@@ -29581,7 +29804,7 @@
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A348" s="0" t="s">
+      <c r="A348" s="1" t="s">
         <v>7474</v>
       </c>
       <c r="B348" s="1" t="s">
@@ -29589,7 +29812,7 @@
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A349" s="0" t="s">
+      <c r="A349" s="1" t="s">
         <v>7476</v>
       </c>
       <c r="B349" s="1" t="s">
@@ -29597,7 +29820,7 @@
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A350" s="0" t="s">
+      <c r="A350" s="1" t="s">
         <v>7478</v>
       </c>
       <c r="B350" s="1" t="s">
@@ -29605,7 +29828,7 @@
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="0" t="s">
+      <c r="A351" s="1" t="s">
         <v>7480</v>
       </c>
       <c r="B351" s="1" t="s">
@@ -29613,7 +29836,7 @@
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A352" s="0" t="s">
+      <c r="A352" s="1" t="s">
         <v>7482</v>
       </c>
       <c r="B352" s="1" t="s">
@@ -29621,7 +29844,7 @@
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A353" s="0" t="s">
+      <c r="A353" s="1" t="s">
         <v>7484</v>
       </c>
       <c r="B353" s="1" t="s">
@@ -29629,7 +29852,7 @@
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="0" t="s">
+      <c r="A354" s="1" t="s">
         <v>7486</v>
       </c>
       <c r="B354" s="1" t="s">
@@ -29637,7 +29860,7 @@
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="0" t="s">
+      <c r="A355" s="1" t="s">
         <v>7488</v>
       </c>
       <c r="B355" s="1" t="s">
@@ -29645,7 +29868,7 @@
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="0" t="s">
+      <c r="A356" s="1" t="s">
         <v>7490</v>
       </c>
       <c r="B356" s="1" t="s">
@@ -29653,7 +29876,7 @@
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="0" t="s">
+      <c r="A357" s="1" t="s">
         <v>7492</v>
       </c>
       <c r="B357" s="1" t="s">
@@ -29661,7 +29884,7 @@
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A358" s="0" t="s">
+      <c r="A358" s="1" t="s">
         <v>7494</v>
       </c>
       <c r="B358" s="1" t="s">
@@ -29669,7 +29892,7 @@
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="0" t="s">
+      <c r="A359" s="1" t="s">
         <v>7496</v>
       </c>
       <c r="B359" s="1" t="s">
@@ -29677,7 +29900,7 @@
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A360" s="0" t="s">
+      <c r="A360" s="1" t="s">
         <v>7498</v>
       </c>
       <c r="B360" s="1" t="s">
@@ -29685,7 +29908,7 @@
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A361" s="0" t="s">
+      <c r="A361" s="1" t="s">
         <v>7500</v>
       </c>
       <c r="B361" s="1" t="s">
@@ -29693,7 +29916,7 @@
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A362" s="0" t="s">
+      <c r="A362" s="1" t="s">
         <v>7502</v>
       </c>
       <c r="B362" s="1" t="s">
@@ -29701,7 +29924,7 @@
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A363" s="0" t="s">
+      <c r="A363" s="1" t="s">
         <v>7504</v>
       </c>
       <c r="B363" s="1" t="s">
@@ -29709,7 +29932,7 @@
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A364" s="0" t="s">
+      <c r="A364" s="1" t="s">
         <v>7506</v>
       </c>
       <c r="B364" s="1" t="s">
@@ -29717,7 +29940,7 @@
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A365" s="0" t="s">
+      <c r="A365" s="1" t="s">
         <v>7508</v>
       </c>
       <c r="B365" s="1" t="s">
@@ -29725,7 +29948,7 @@
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A366" s="0" t="s">
+      <c r="A366" s="1" t="s">
         <v>7510</v>
       </c>
       <c r="B366" s="1" t="s">
@@ -29733,7 +29956,7 @@
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A367" s="0" t="s">
+      <c r="A367" s="1" t="s">
         <v>7512</v>
       </c>
       <c r="B367" s="1" t="s">
@@ -29741,7 +29964,7 @@
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A368" s="0" t="s">
+      <c r="A368" s="1" t="s">
         <v>7514</v>
       </c>
       <c r="B368" s="1" t="s">
@@ -29749,7 +29972,7 @@
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A369" s="0" t="s">
+      <c r="A369" s="1" t="s">
         <v>7516</v>
       </c>
       <c r="B369" s="1" t="s">
@@ -29757,7 +29980,7 @@
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A370" s="0" t="s">
+      <c r="A370" s="1" t="s">
         <v>7518</v>
       </c>
       <c r="B370" s="1" t="s">
@@ -29765,7 +29988,7 @@
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A371" s="0" t="s">
+      <c r="A371" s="1" t="s">
         <v>7520</v>
       </c>
       <c r="B371" s="1" t="s">
@@ -29773,7 +29996,7 @@
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A372" s="0" t="s">
+      <c r="A372" s="1" t="s">
         <v>7522</v>
       </c>
       <c r="B372" s="1" t="s">
@@ -29781,7 +30004,7 @@
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="0" t="s">
+      <c r="A373" s="1" t="s">
         <v>7524</v>
       </c>
       <c r="B373" s="1" t="s">
@@ -29789,7 +30012,7 @@
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="0" t="s">
+      <c r="A374" s="1" t="s">
         <v>7526</v>
       </c>
       <c r="B374" s="1" t="s">
@@ -29797,7 +30020,7 @@
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A375" s="0" t="s">
+      <c r="A375" s="1" t="s">
         <v>7528</v>
       </c>
       <c r="B375" s="1" t="s">
@@ -29805,7 +30028,7 @@
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A376" s="0" t="s">
+      <c r="A376" s="1" t="s">
         <v>7530</v>
       </c>
       <c r="B376" s="1" t="s">
@@ -29813,7 +30036,7 @@
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A377" s="0" t="s">
+      <c r="A377" s="1" t="s">
         <v>7532</v>
       </c>
       <c r="B377" s="1" t="s">
@@ -29821,7 +30044,7 @@
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A378" s="0" t="s">
+      <c r="A378" s="1" t="s">
         <v>7534</v>
       </c>
       <c r="B378" s="1" t="s">
@@ -29829,7 +30052,7 @@
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="0" t="s">
+      <c r="A379" s="1" t="s">
         <v>7536</v>
       </c>
       <c r="B379" s="1" t="s">
@@ -29837,7 +30060,7 @@
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="0" t="s">
+      <c r="A380" s="1" t="s">
         <v>7538</v>
       </c>
       <c r="B380" s="1" t="s">
@@ -29845,7 +30068,7 @@
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="0" t="s">
+      <c r="A381" s="1" t="s">
         <v>7540</v>
       </c>
       <c r="B381" s="1" t="s">
@@ -29853,7 +30076,7 @@
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="0" t="s">
+      <c r="A382" s="1" t="s">
         <v>7542</v>
       </c>
       <c r="B382" s="1" t="s">
@@ -29861,7 +30084,7 @@
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="0" t="s">
+      <c r="A383" s="1" t="s">
         <v>7544</v>
       </c>
       <c r="B383" s="1" t="s">
@@ -29869,7 +30092,7 @@
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="0" t="s">
+      <c r="A384" s="1" t="s">
         <v>7546</v>
       </c>
       <c r="B384" s="1" t="s">
@@ -29877,7 +30100,7 @@
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A385" s="0" t="s">
+      <c r="A385" s="1" t="s">
         <v>7548</v>
       </c>
       <c r="B385" s="1" t="s">
@@ -29885,7 +30108,7 @@
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A386" s="0" t="s">
+      <c r="A386" s="1" t="s">
         <v>7550</v>
       </c>
       <c r="B386" s="1" t="s">
@@ -29893,7 +30116,7 @@
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="0" t="s">
+      <c r="A387" s="1" t="s">
         <v>7552</v>
       </c>
       <c r="B387" s="1" t="s">
@@ -29901,7 +30124,7 @@
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="0" t="s">
+      <c r="A388" s="1" t="s">
         <v>7554</v>
       </c>
       <c r="B388" s="1" t="s">
@@ -29909,7 +30132,7 @@
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="0" t="s">
+      <c r="A389" s="1" t="s">
         <v>7556</v>
       </c>
       <c r="B389" s="1" t="s">
@@ -29917,7 +30140,7 @@
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A390" s="0" t="s">
+      <c r="A390" s="1" t="s">
         <v>7558</v>
       </c>
       <c r="B390" s="1" t="s">
@@ -29925,7 +30148,7 @@
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A391" s="0" t="s">
+      <c r="A391" s="1" t="s">
         <v>7560</v>
       </c>
       <c r="B391" s="1" t="s">
@@ -29933,7 +30156,7 @@
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A392" s="0" t="s">
+      <c r="A392" s="1" t="s">
         <v>7562</v>
       </c>
       <c r="B392" s="1" t="s">
@@ -29941,7 +30164,7 @@
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A393" s="0" t="s">
+      <c r="A393" s="1" t="s">
         <v>7564</v>
       </c>
       <c r="B393" s="1" t="s">
@@ -29949,7 +30172,7 @@
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A394" s="0" t="s">
+      <c r="A394" s="1" t="s">
         <v>7566</v>
       </c>
       <c r="B394" s="1" t="s">
@@ -29957,7 +30180,7 @@
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A395" s="0" t="s">
+      <c r="A395" s="1" t="s">
         <v>7568</v>
       </c>
       <c r="B395" s="1" t="s">
@@ -29965,7 +30188,7 @@
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A396" s="0" t="s">
+      <c r="A396" s="1" t="s">
         <v>7570</v>
       </c>
       <c r="B396" s="1" t="s">
@@ -29973,7 +30196,7 @@
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A397" s="0" t="s">
+      <c r="A397" s="1" t="s">
         <v>7572</v>
       </c>
       <c r="B397" s="1" t="s">
@@ -29981,7 +30204,7 @@
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A398" s="0" t="s">
+      <c r="A398" s="1" t="s">
         <v>7574</v>
       </c>
       <c r="B398" s="1" t="s">
@@ -29989,7 +30212,7 @@
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A399" s="0" t="s">
+      <c r="A399" s="1" t="s">
         <v>7576</v>
       </c>
       <c r="B399" s="1" t="s">
@@ -29997,7 +30220,7 @@
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A400" s="0" t="s">
+      <c r="A400" s="1" t="s">
         <v>7578</v>
       </c>
       <c r="B400" s="1" t="s">
@@ -30005,7 +30228,7 @@
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="0" t="s">
+      <c r="A401" s="1" t="s">
         <v>7580</v>
       </c>
       <c r="B401" s="1" t="s">
@@ -30013,7 +30236,7 @@
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="0" t="s">
+      <c r="A402" s="1" t="s">
         <v>7582</v>
       </c>
       <c r="B402" s="1" t="s">
@@ -30021,7 +30244,7 @@
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="0" t="s">
+      <c r="A403" s="1" t="s">
         <v>7584</v>
       </c>
       <c r="B403" s="1" t="s">
@@ -30029,7 +30252,7 @@
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A404" s="0" t="s">
+      <c r="A404" s="1" t="s">
         <v>7586</v>
       </c>
       <c r="B404" s="1" t="s">
@@ -30037,7 +30260,7 @@
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="0" t="s">
+      <c r="A405" s="1" t="s">
         <v>7588</v>
       </c>
       <c r="B405" s="1" t="s">
@@ -30045,7 +30268,7 @@
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="0" t="s">
+      <c r="A406" s="1" t="s">
         <v>7590</v>
       </c>
       <c r="B406" s="1" t="s">
@@ -30053,7 +30276,7 @@
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="0" t="s">
+      <c r="A407" s="1" t="s">
         <v>7592</v>
       </c>
       <c r="B407" s="1" t="s">
@@ -30061,7 +30284,7 @@
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A408" s="0" t="s">
+      <c r="A408" s="1" t="s">
         <v>7594</v>
       </c>
       <c r="B408" s="1" t="s">
@@ -30069,7 +30292,7 @@
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A409" s="0" t="s">
+      <c r="A409" s="1" t="s">
         <v>7596</v>
       </c>
       <c r="B409" s="1" t="s">
@@ -30077,7 +30300,7 @@
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="0" t="s">
+      <c r="A410" s="1" t="s">
         <v>7598</v>
       </c>
       <c r="B410" s="1" t="s">
@@ -30085,7 +30308,7 @@
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A411" s="0" t="s">
+      <c r="A411" s="1" t="s">
         <v>7600</v>
       </c>
       <c r="B411" s="1" t="s">
@@ -30093,7 +30316,7 @@
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A412" s="0" t="s">
+      <c r="A412" s="1" t="s">
         <v>7602</v>
       </c>
       <c r="B412" s="1" t="s">
@@ -30101,7 +30324,7 @@
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="0" t="s">
+      <c r="A413" s="1" t="s">
         <v>7604</v>
       </c>
       <c r="B413" s="1" t="s">
@@ -30109,7 +30332,7 @@
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="0" t="s">
+      <c r="A414" s="1" t="s">
         <v>7606</v>
       </c>
       <c r="B414" s="1" t="s">
@@ -30117,7 +30340,7 @@
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="0" t="s">
+      <c r="A415" s="1" t="s">
         <v>7608</v>
       </c>
       <c r="B415" s="1" t="s">
@@ -30125,7 +30348,7 @@
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A416" s="0" t="s">
+      <c r="A416" s="1" t="s">
         <v>7610</v>
       </c>
       <c r="B416" s="1" t="s">
@@ -30133,7 +30356,7 @@
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A417" s="0" t="s">
+      <c r="A417" s="1" t="s">
         <v>7612</v>
       </c>
       <c r="B417" s="1" t="s">
@@ -30141,7 +30364,7 @@
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A418" s="0" t="s">
+      <c r="A418" s="1" t="s">
         <v>7614</v>
       </c>
       <c r="B418" s="1" t="s">
@@ -30149,7 +30372,7 @@
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A419" s="0" t="s">
+      <c r="A419" s="1" t="s">
         <v>7616</v>
       </c>
       <c r="B419" s="1" t="s">
@@ -30157,7 +30380,7 @@
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="0" t="s">
+      <c r="A420" s="1" t="s">
         <v>7618</v>
       </c>
       <c r="B420" s="1" t="s">
@@ -30165,7 +30388,7 @@
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A421" s="0" t="s">
+      <c r="A421" s="1" t="s">
         <v>7620</v>
       </c>
       <c r="B421" s="1" t="s">
@@ -30173,7 +30396,7 @@
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A422" s="0" t="s">
+      <c r="A422" s="1" t="s">
         <v>7622</v>
       </c>
       <c r="B422" s="1" t="s">
@@ -30181,7 +30404,7 @@
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="0" t="s">
+      <c r="A423" s="1" t="s">
         <v>7624</v>
       </c>
       <c r="B423" s="1" t="s">
@@ -30189,7 +30412,7 @@
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="0" t="s">
+      <c r="A424" s="1" t="s">
         <v>7626</v>
       </c>
       <c r="B424" s="1" t="s">
@@ -30197,7 +30420,7 @@
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A425" s="0" t="s">
+      <c r="A425" s="1" t="s">
         <v>1859</v>
       </c>
       <c r="B425" s="1" t="s">
@@ -30205,7 +30428,7 @@
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A426" s="0" t="s">
+      <c r="A426" s="1" t="s">
         <v>7628</v>
       </c>
       <c r="B426" s="1" t="s">
@@ -30213,7 +30436,7 @@
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A427" s="0" t="s">
+      <c r="A427" s="1" t="s">
         <v>7630</v>
       </c>
       <c r="B427" s="1" t="s">
@@ -30221,7 +30444,7 @@
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A428" s="0" t="s">
+      <c r="A428" s="1" t="s">
         <v>7632</v>
       </c>
       <c r="B428" s="1" t="s">
@@ -30229,7 +30452,7 @@
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="0" t="s">
+      <c r="A429" s="1" t="s">
         <v>7634</v>
       </c>
       <c r="B429" s="1" t="s">
@@ -30237,7 +30460,7 @@
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="0" t="s">
+      <c r="A430" s="1" t="s">
         <v>7636</v>
       </c>
       <c r="B430" s="1" t="s">
@@ -30245,7 +30468,7 @@
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="0" t="s">
+      <c r="A431" s="1" t="s">
         <v>7638</v>
       </c>
       <c r="B431" s="1" t="s">
@@ -30253,7 +30476,7 @@
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="0" t="s">
+      <c r="A432" s="1" t="s">
         <v>7640</v>
       </c>
       <c r="B432" s="1" t="s">
@@ -30261,7 +30484,7 @@
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="0" t="s">
+      <c r="A433" s="1" t="s">
         <v>7642</v>
       </c>
       <c r="B433" s="1" t="s">
@@ -30269,7 +30492,7 @@
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="0" t="s">
+      <c r="A434" s="1" t="s">
         <v>7644</v>
       </c>
       <c r="B434" s="1" t="s">
@@ -30277,7 +30500,7 @@
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="0" t="s">
+      <c r="A435" s="1" t="s">
         <v>7646</v>
       </c>
       <c r="B435" s="1" t="s">
@@ -30285,7 +30508,7 @@
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="0" t="s">
+      <c r="A436" s="1" t="s">
         <v>7648</v>
       </c>
       <c r="B436" s="1" t="s">
@@ -30293,7 +30516,7 @@
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="0" t="s">
+      <c r="A437" s="1" t="s">
         <v>7650</v>
       </c>
       <c r="B437" s="1" t="s">
@@ -30301,7 +30524,7 @@
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="0" t="s">
+      <c r="A438" s="1" t="s">
         <v>7652</v>
       </c>
       <c r="B438" s="1" t="s">
@@ -30309,7 +30532,7 @@
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="0" t="s">
+      <c r="A439" s="1" t="s">
         <v>7654</v>
       </c>
       <c r="B439" s="1" t="s">
@@ -30317,7 +30540,7 @@
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="0" t="s">
+      <c r="A440" s="1" t="s">
         <v>7656</v>
       </c>
       <c r="B440" s="1" t="s">
@@ -30325,7 +30548,7 @@
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="0" t="s">
+      <c r="A441" s="1" t="s">
         <v>7658</v>
       </c>
       <c r="B441" s="1" t="s">
@@ -30333,7 +30556,7 @@
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="0" t="s">
+      <c r="A442" s="1" t="s">
         <v>7660</v>
       </c>
       <c r="B442" s="1" t="s">
@@ -30341,7 +30564,7 @@
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="0" t="s">
+      <c r="A443" s="1" t="s">
         <v>7662</v>
       </c>
       <c r="B443" s="1" t="s">
@@ -30349,7 +30572,7 @@
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="0" t="s">
+      <c r="A444" s="1" t="s">
         <v>7664</v>
       </c>
       <c r="B444" s="1" t="s">
@@ -30357,7 +30580,7 @@
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A445" s="0" t="s">
+      <c r="A445" s="1" t="s">
         <v>7666</v>
       </c>
       <c r="B445" s="1" t="s">
@@ -30365,7 +30588,7 @@
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="0" t="s">
+      <c r="A446" s="1" t="s">
         <v>7668</v>
       </c>
       <c r="B446" s="1" t="s">
@@ -30373,7 +30596,7 @@
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A447" s="0" t="s">
+      <c r="A447" s="1" t="s">
         <v>7670</v>
       </c>
       <c r="B447" s="1" t="s">
@@ -30381,7 +30604,7 @@
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="0" t="s">
+      <c r="A448" s="1" t="s">
         <v>7672</v>
       </c>
       <c r="B448" s="1" t="s">
@@ -30389,7 +30612,7 @@
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="0" t="s">
+      <c r="A449" s="1" t="s">
         <v>7674</v>
       </c>
       <c r="B449" s="1" t="s">
@@ -30397,7 +30620,7 @@
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="0" t="s">
+      <c r="A450" s="1" t="s">
         <v>7676</v>
       </c>
       <c r="B450" s="1" t="s">
@@ -30405,7 +30628,7 @@
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="0" t="s">
+      <c r="A451" s="1" t="s">
         <v>7678</v>
       </c>
       <c r="B451" s="1" t="s">
@@ -30413,7 +30636,7 @@
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A452" s="0" t="s">
+      <c r="A452" s="1" t="s">
         <v>7680</v>
       </c>
       <c r="B452" s="1" t="s">
@@ -30421,7 +30644,7 @@
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="0" t="s">
+      <c r="A453" s="1" t="s">
         <v>7682</v>
       </c>
       <c r="B453" s="1" t="s">
@@ -30429,7 +30652,7 @@
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A454" s="0" t="s">
+      <c r="A454" s="1" t="s">
         <v>7684</v>
       </c>
       <c r="B454" s="1" t="s">
@@ -30437,7 +30660,7 @@
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A455" s="0" t="s">
+      <c r="A455" s="1" t="s">
         <v>7686</v>
       </c>
       <c r="B455" s="1" t="s">
@@ -30445,7 +30668,7 @@
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A456" s="0" t="s">
+      <c r="A456" s="1" t="s">
         <v>7688</v>
       </c>
       <c r="B456" s="1" t="s">
@@ -30453,7 +30676,7 @@
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A457" s="0" t="s">
+      <c r="A457" s="1" t="s">
         <v>7690</v>
       </c>
       <c r="B457" s="1" t="s">
@@ -30461,7 +30684,7 @@
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="0" t="s">
+      <c r="A458" s="1" t="s">
         <v>7692</v>
       </c>
       <c r="B458" s="1" t="s">
@@ -30469,7 +30692,7 @@
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="0" t="s">
+      <c r="A459" s="1" t="s">
         <v>7694</v>
       </c>
       <c r="B459" s="1" t="s">
@@ -30477,7 +30700,7 @@
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="0" t="s">
+      <c r="A460" s="1" t="s">
         <v>7696</v>
       </c>
       <c r="B460" s="1" t="s">
@@ -30485,7 +30708,7 @@
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A461" s="0" t="s">
+      <c r="A461" s="1" t="s">
         <v>7698</v>
       </c>
       <c r="B461" s="1" t="s">
@@ -30493,7 +30716,7 @@
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A462" s="0" t="s">
+      <c r="A462" s="1" t="s">
         <v>7700</v>
       </c>
       <c r="B462" s="1" t="s">
@@ -30501,7 +30724,7 @@
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A463" s="0" t="s">
+      <c r="A463" s="1" t="s">
         <v>7702</v>
       </c>
       <c r="B463" s="1" t="s">
@@ -30509,7 +30732,7 @@
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A464" s="0" t="s">
+      <c r="A464" s="1" t="s">
         <v>7704</v>
       </c>
       <c r="B464" s="1" t="s">
@@ -30517,7 +30740,7 @@
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="0" t="s">
+      <c r="A465" s="1" t="s">
         <v>7706</v>
       </c>
       <c r="B465" s="1" t="s">
@@ -30525,7 +30748,7 @@
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A466" s="0" t="s">
+      <c r="A466" s="1" t="s">
         <v>7708</v>
       </c>
       <c r="B466" s="1" t="s">
@@ -30533,7 +30756,7 @@
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A467" s="0" t="s">
+      <c r="A467" s="1" t="s">
         <v>7710</v>
       </c>
       <c r="B467" s="1" t="s">
@@ -30541,7 +30764,7 @@
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A468" s="0" t="s">
+      <c r="A468" s="1" t="s">
         <v>7712</v>
       </c>
       <c r="B468" s="1" t="s">
@@ -30549,7 +30772,7 @@
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A469" s="0" t="s">
+      <c r="A469" s="1" t="s">
         <v>7714</v>
       </c>
       <c r="B469" s="1" t="s">
@@ -30557,7 +30780,7 @@
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="0" t="s">
+      <c r="A470" s="1" t="s">
         <v>7716</v>
       </c>
       <c r="B470" s="1" t="s">
@@ -30565,7 +30788,7 @@
       </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A471" s="0" t="s">
+      <c r="A471" s="1" t="s">
         <v>7718</v>
       </c>
       <c r="B471" s="1" t="s">
@@ -30573,7 +30796,7 @@
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="0" t="s">
+      <c r="A472" s="1" t="s">
         <v>7720</v>
       </c>
       <c r="B472" s="1" t="s">
@@ -30581,7 +30804,7 @@
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="0" t="s">
+      <c r="A473" s="1" t="s">
         <v>7722</v>
       </c>
       <c r="B473" s="1" t="s">
@@ -30589,7 +30812,7 @@
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="0" t="s">
+      <c r="A474" s="1" t="s">
         <v>7724</v>
       </c>
       <c r="B474" s="1" t="s">
@@ -30597,7 +30820,7 @@
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="0" t="s">
+      <c r="A475" s="1" t="s">
         <v>7726</v>
       </c>
       <c r="B475" s="1" t="s">
@@ -30605,7 +30828,7 @@
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A476" s="0" t="s">
+      <c r="A476" s="1" t="s">
         <v>7728</v>
       </c>
       <c r="B476" s="1" t="s">
@@ -30613,7 +30836,7 @@
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="0" t="s">
+      <c r="A477" s="1" t="s">
         <v>7730</v>
       </c>
       <c r="B477" s="1" t="s">
@@ -30621,7 +30844,7 @@
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="0" t="s">
+      <c r="A478" s="1" t="s">
         <v>7732</v>
       </c>
       <c r="B478" s="1" t="s">
@@ -30629,7 +30852,7 @@
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="0" t="s">
+      <c r="A479" s="1" t="s">
         <v>7734</v>
       </c>
       <c r="B479" s="1" t="s">
@@ -30637,7 +30860,7 @@
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="0" t="s">
+      <c r="A480" s="1" t="s">
         <v>7736</v>
       </c>
       <c r="B480" s="1" t="s">
@@ -30645,7 +30868,7 @@
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A481" s="0" t="s">
+      <c r="A481" s="1" t="s">
         <v>7738</v>
       </c>
       <c r="B481" s="1" t="s">
@@ -30653,7 +30876,7 @@
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="0" t="s">
+      <c r="A482" s="1" t="s">
         <v>7740</v>
       </c>
       <c r="B482" s="1" t="s">
@@ -30661,7 +30884,7 @@
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A483" s="0" t="s">
+      <c r="A483" s="1" t="s">
         <v>7742</v>
       </c>
       <c r="B483" s="1" t="s">
@@ -30669,7 +30892,7 @@
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A484" s="0" t="s">
+      <c r="A484" s="1" t="s">
         <v>7744</v>
       </c>
       <c r="B484" s="1" t="s">
@@ -30677,7 +30900,7 @@
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A485" s="0" t="s">
+      <c r="A485" s="1" t="s">
         <v>7746</v>
       </c>
       <c r="B485" s="1" t="s">
@@ -30685,7 +30908,7 @@
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A486" s="0" t="s">
+      <c r="A486" s="1" t="s">
         <v>7748</v>
       </c>
       <c r="B486" s="1" t="s">
@@ -30693,7 +30916,7 @@
       </c>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="0" t="s">
+      <c r="A487" s="1" t="s">
         <v>7750</v>
       </c>
       <c r="B487" s="1" t="s">
@@ -30701,7 +30924,7 @@
       </c>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A488" s="0" t="s">
+      <c r="A488" s="1" t="s">
         <v>7752</v>
       </c>
       <c r="B488" s="1" t="s">
@@ -30709,7 +30932,7 @@
       </c>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A489" s="0" t="s">
+      <c r="A489" s="1" t="s">
         <v>7754</v>
       </c>
       <c r="B489" s="1" t="s">
@@ -30717,7 +30940,7 @@
       </c>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A490" s="0" t="s">
+      <c r="A490" s="1" t="s">
         <v>7756</v>
       </c>
       <c r="B490" s="1" t="s">
@@ -30725,7 +30948,7 @@
       </c>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A491" s="0" t="s">
+      <c r="A491" s="1" t="s">
         <v>7758</v>
       </c>
       <c r="B491" s="1" t="s">
@@ -30733,7 +30956,7 @@
       </c>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A492" s="0" t="s">
+      <c r="A492" s="1" t="s">
         <v>7760</v>
       </c>
       <c r="B492" s="1" t="s">
@@ -30741,7 +30964,7 @@
       </c>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="0" t="s">
+      <c r="A493" s="1" t="s">
         <v>7762</v>
       </c>
       <c r="B493" s="1" t="s">
@@ -30749,7 +30972,7 @@
       </c>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A494" s="0" t="s">
+      <c r="A494" s="1" t="s">
         <v>7764</v>
       </c>
       <c r="B494" s="1" t="s">
@@ -30757,7 +30980,7 @@
       </c>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A495" s="0" t="s">
+      <c r="A495" s="1" t="s">
         <v>7766</v>
       </c>
       <c r="B495" s="1" t="s">
@@ -30765,7 +30988,7 @@
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A496" s="0" t="s">
+      <c r="A496" s="1" t="s">
         <v>7768</v>
       </c>
       <c r="B496" s="1" t="s">
@@ -30773,7 +30996,7 @@
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A497" s="0" t="s">
+      <c r="A497" s="1" t="s">
         <v>7770</v>
       </c>
       <c r="B497" s="1" t="s">
@@ -30781,7 +31004,7 @@
       </c>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A498" s="0" t="s">
+      <c r="A498" s="1" t="s">
         <v>7772</v>
       </c>
       <c r="B498" s="1" t="s">
@@ -30789,7 +31012,7 @@
       </c>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="0" t="s">
+      <c r="A499" s="1" t="s">
         <v>7774</v>
       </c>
       <c r="B499" s="1" t="s">
@@ -30797,7 +31020,7 @@
       </c>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A500" s="0" t="s">
+      <c r="A500" s="1" t="s">
         <v>7776</v>
       </c>
       <c r="B500" s="1" t="s">
@@ -30805,7 +31028,7 @@
       </c>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A501" s="0" t="s">
+      <c r="A501" s="1" t="s">
         <v>7778</v>
       </c>
       <c r="B501" s="1" t="s">
@@ -30813,7 +31036,7 @@
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A502" s="0" t="s">
+      <c r="A502" s="1" t="s">
         <v>7780</v>
       </c>
       <c r="B502" s="1" t="s">
@@ -30821,7 +31044,7 @@
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A503" s="0" t="s">
+      <c r="A503" s="1" t="s">
         <v>7782</v>
       </c>
       <c r="B503" s="1" t="s">
@@ -30829,7 +31052,7 @@
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A504" s="0" t="s">
+      <c r="A504" s="1" t="s">
         <v>7784</v>
       </c>
       <c r="B504" s="1" t="s">
@@ -30837,7 +31060,7 @@
       </c>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="0" t="s">
+      <c r="A505" s="1" t="s">
         <v>7786</v>
       </c>
       <c r="B505" s="1" t="s">
@@ -30845,7 +31068,7 @@
       </c>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A506" s="0" t="s">
+      <c r="A506" s="1" t="s">
         <v>7788</v>
       </c>
       <c r="B506" s="1" t="s">
@@ -30853,7 +31076,7 @@
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A507" s="0" t="s">
+      <c r="A507" s="1" t="s">
         <v>7790</v>
       </c>
       <c r="B507" s="1" t="s">
@@ -30861,7 +31084,7 @@
       </c>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A508" s="0" t="s">
+      <c r="A508" s="1" t="s">
         <v>7792</v>
       </c>
       <c r="B508" s="1" t="s">
@@ -30869,7 +31092,7 @@
       </c>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A509" s="0" t="s">
+      <c r="A509" s="1" t="s">
         <v>7794</v>
       </c>
       <c r="B509" s="1" t="s">
@@ -30877,7 +31100,7 @@
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A510" s="0" t="s">
+      <c r="A510" s="1" t="s">
         <v>7796</v>
       </c>
       <c r="B510" s="1" t="s">
@@ -30885,7 +31108,7 @@
       </c>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A511" s="0" t="s">
+      <c r="A511" s="1" t="s">
         <v>7798</v>
       </c>
       <c r="B511" s="1" t="s">
@@ -30893,7 +31116,7 @@
       </c>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A512" s="0" t="s">
+      <c r="A512" s="1" t="s">
         <v>7800</v>
       </c>
       <c r="B512" s="1" t="s">
@@ -30901,7 +31124,7 @@
       </c>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A513" s="0" t="s">
+      <c r="A513" s="1" t="s">
         <v>7802</v>
       </c>
       <c r="B513" s="1" t="s">
@@ -30909,7 +31132,7 @@
       </c>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A514" s="0" t="s">
+      <c r="A514" s="1" t="s">
         <v>7804</v>
       </c>
       <c r="B514" s="1" t="s">
@@ -30917,7 +31140,7 @@
       </c>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A515" s="0" t="s">
+      <c r="A515" s="1" t="s">
         <v>7806</v>
       </c>
       <c r="B515" s="1" t="s">
@@ -30925,7 +31148,7 @@
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A516" s="0" t="s">
+      <c r="A516" s="1" t="s">
         <v>7808</v>
       </c>
       <c r="B516" s="1" t="s">
@@ -30933,7 +31156,7 @@
       </c>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A517" s="0" t="s">
+      <c r="A517" s="1" t="s">
         <v>7810</v>
       </c>
       <c r="B517" s="1" t="s">
@@ -30941,7 +31164,7 @@
       </c>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A518" s="0" t="s">
+      <c r="A518" s="1" t="s">
         <v>7812</v>
       </c>
       <c r="B518" s="1" t="s">
@@ -30949,7 +31172,7 @@
       </c>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A519" s="0" t="s">
+      <c r="A519" s="1" t="s">
         <v>7814</v>
       </c>
       <c r="B519" s="1" t="s">
@@ -30957,7 +31180,7 @@
       </c>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A520" s="0" t="s">
+      <c r="A520" s="1" t="s">
         <v>7816</v>
       </c>
       <c r="B520" s="1" t="s">
@@ -30965,7 +31188,7 @@
       </c>
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A521" s="0" t="s">
+      <c r="A521" s="1" t="s">
         <v>7818</v>
       </c>
       <c r="B521" s="1" t="s">
@@ -30973,7 +31196,7 @@
       </c>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A522" s="0" t="s">
+      <c r="A522" s="1" t="s">
         <v>7820</v>
       </c>
       <c r="B522" s="1" t="s">
@@ -30981,7 +31204,7 @@
       </c>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="0" t="s">
+      <c r="A523" s="1" t="s">
         <v>7822</v>
       </c>
       <c r="B523" s="1" t="s">
@@ -30989,7 +31212,7 @@
       </c>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A524" s="0" t="s">
+      <c r="A524" s="1" t="s">
         <v>7824</v>
       </c>
       <c r="B524" s="1" t="s">
@@ -30997,7 +31220,7 @@
       </c>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A525" s="0" t="s">
+      <c r="A525" s="1" t="s">
         <v>7826</v>
       </c>
       <c r="B525" s="1" t="s">
@@ -31005,7 +31228,7 @@
       </c>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A526" s="0" t="s">
+      <c r="A526" s="1" t="s">
         <v>7828</v>
       </c>
       <c r="B526" s="1" t="s">
@@ -31013,7 +31236,7 @@
       </c>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="0" t="s">
+      <c r="A527" s="1" t="s">
         <v>7830</v>
       </c>
       <c r="B527" s="1" t="s">
@@ -31021,7 +31244,7 @@
       </c>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A528" s="0" t="s">
+      <c r="A528" s="1" t="s">
         <v>7832</v>
       </c>
       <c r="B528" s="1" t="s">
@@ -31029,7 +31252,7 @@
       </c>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A529" s="0" t="s">
+      <c r="A529" s="1" t="s">
         <v>7834</v>
       </c>
       <c r="B529" s="1" t="s">
@@ -31037,7 +31260,7 @@
       </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A530" s="0" t="s">
+      <c r="A530" s="1" t="s">
         <v>7836</v>
       </c>
       <c r="B530" s="1" t="s">
@@ -31045,7 +31268,7 @@
       </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A531" s="0" t="s">
+      <c r="A531" s="1" t="s">
         <v>7838</v>
       </c>
       <c r="B531" s="1" t="s">
@@ -31053,7 +31276,7 @@
       </c>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="0" t="s">
+      <c r="A532" s="1" t="s">
         <v>7840</v>
       </c>
       <c r="B532" s="1" t="s">
@@ -31061,7 +31284,7 @@
       </c>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A533" s="0" t="s">
+      <c r="A533" s="1" t="s">
         <v>7842</v>
       </c>
       <c r="B533" s="1" t="s">
@@ -31069,7 +31292,7 @@
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A534" s="0" t="s">
+      <c r="A534" s="1" t="s">
         <v>7844</v>
       </c>
       <c r="B534" s="1" t="s">
@@ -31077,7 +31300,7 @@
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A535" s="0" t="s">
+      <c r="A535" s="1" t="s">
         <v>7846</v>
       </c>
       <c r="B535" s="1" t="s">
@@ -31085,7 +31308,7 @@
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A536" s="0" t="s">
+      <c r="A536" s="1" t="s">
         <v>7848</v>
       </c>
       <c r="B536" s="1" t="s">
@@ -31093,7 +31316,7 @@
       </c>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="0" t="s">
+      <c r="A537" s="1" t="s">
         <v>7850</v>
       </c>
       <c r="B537" s="1" t="s">
@@ -31101,11 +31324,343 @@
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A538" s="0" t="s">
+      <c r="A538" s="1" t="s">
         <v>7852</v>
       </c>
       <c r="B538" s="1" t="s">
         <v>7853</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.74"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7854</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7855</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7856</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7857</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7858</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7859</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7860</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7861</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>7862</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7863</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>7864</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7865</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>7866</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7867</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>7868</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7869</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>7870</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7871</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>7872</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7873</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>7874</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7875</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>7876</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7877</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>7878</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7879</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>7880</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7881</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>7882</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7883</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>7884</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7885</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>7886</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7887</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>7888</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7889</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>7890</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7891</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>7892</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7893</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>7894</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7895</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>7896</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7897</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>7898</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7899</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>7900</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7901</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>7902</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7903</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>7904</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7905</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>7906</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7907</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>7908</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7909</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>7910</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7911</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>7912</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7913</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>7914</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7915</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>7916</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7917</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>7918</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7919</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>7920</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7921</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>7922</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7923</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>7924</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7925</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>7926</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "YuryodoYomikataJiten" sheet in "OtoYakuNoHeyaYomikataJiten.xlsx" file Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenYuryodoYomikataJitenMultimapFactoryBean.sheetName" property in "configuration.properties" Extends "org.springframework.beans.factory.StringMultiMapFromResourceFactoryBean" class by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenYuryodoYomikataJitenMultimapFactoryBean" Class Update "applicationContext.xml" Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenYuryodoYomikataJitenMultimapFactoryBean.getObject()" method
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -19,6 +19,7 @@
     <sheet name="JRSenYomikataJiten" sheetId="9" state="visible" r:id="rId11"/>
     <sheet name="MintetsuYomikataJiten" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="SintomeiYomikataJiten" sheetId="11" state="visible" r:id="rId13"/>
+    <sheet name="YuryodoYomikataJiten" sheetId="12" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8502" uniqueCount="7928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8984" uniqueCount="8398">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -25165,6 +25166,1416 @@
   </si>
   <si>
     <t xml:space="preserve">しんとうめいこうそくどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">藻岩山観光自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もいわやまかんこうじどうしゃどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">第二</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいに</t>
+  </si>
+  <si>
+    <t xml:space="preserve">青森中央大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あおもりちゅうおうおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">青森空港有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あおもりくうこうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津軽岩木</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つがるいわき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三陸自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんりくじどうしゃどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仙台松島道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せんだいまつしまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仙台南部道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せんだいなんぶどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日和大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひよりおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">牧山道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まきやまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蔵王</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ざおう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淀川河辺有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よどがわかわべゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西蔵王高原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしざおうこうげん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">羽黒山自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はぐろさんじどうしゃどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湯殿山自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆどのさんじどうしゃどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西吾妻</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしあづま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">磐梯山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばんだいさん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">磐梯吾妻</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばんだいあづま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">母成</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ぼなり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">那須甲子有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なすかしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">霧降高原有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きりふりこうげんゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日塩道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にちえんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鬼怒川道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きぬがわどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">那須高原道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なすこうげんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇都宮鹿沼道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うつのみやかぬまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水郷有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すいごうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浦大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うらおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新大利根橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんおおとねばしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石岡有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いしおかゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">筑波</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つくば</t>
+  </si>
+  <si>
+    <t xml:space="preserve">表筑波</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おもてつくば</t>
+  </si>
+  <si>
+    <t xml:space="preserve">下総利根大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しもうさとねおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日立有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひたちゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水海道有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みつかいどうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">常陸那珂有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひたちなかゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">万座</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まんざ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">万座温泉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まんざおんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みはら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">峰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちゃや</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三才山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みさやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松本</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつもと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新和田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんわだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茅野有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちのゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">平井寺</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひらいじ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">志賀中野有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しがなかのゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白馬長野有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はくばながのゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">五輪大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごりんおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">峰有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みねゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白糸</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しらいと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">妙義荒船林道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みょうぎあらふねりんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">上高地乗鞍林道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かみこうちのりくらりんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蓼科</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たてしな</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林道夢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">りんどうゆめ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">平線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいらせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鹿曲川林道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かくまがわりんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">原林道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はらりんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">林道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">りんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">熊谷東松山有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くまがやひがしまつやまゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富士見川越有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじみかわごえゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">狭山環状有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さやまかんじょうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新浦和橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんうらわばしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新見沼大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんみぬまおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">銚子新大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちょうししんおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">利根</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松戸橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつどばしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松戸三郷有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつどみさとゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松戸野田有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつどのだゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">流山有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながれやまゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">銚子有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちょうしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鴨川有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かもがわゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">勝浦有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かつうらゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">房総</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ぼうそう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千葉外房有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちばそとぼうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">九十九里有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くじゅうくりゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東総有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうそうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東金九十九里有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうがねくじゅうくりゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">稲城大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いなぎおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">逗葉新道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ずようしんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本町山中有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほんちょうやまなかゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三浦縦貫道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みうらじゅうかんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">城</t>
+  </si>
+  <si>
+    <t xml:space="preserve">島大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しまおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湯河原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆがわら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">箱根</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はこね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大観山線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいかんざんせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">十国線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じゅっこくせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">芦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">湖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富士</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河口湖大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かわぐちこおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岳横断道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たけおうだんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">雁坂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かりさか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清里高原道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きよさとこうげんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">立山有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たてやまゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">能越自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のうえつじどうしゃどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有峰林道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ありみねりんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">能登海浜道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のとかいひんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">能登半島縦貫有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のとはんとうじゅうかんゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">川北大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かわきたおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田鶴浜道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たつるはまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はくさん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岳有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だけゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">永平寺有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えいへいじゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河野海岸有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうのかいがんゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">法恩寺山有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほうおんじさんゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三方五湖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みかたごこ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">弁天大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">べんてんおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">村櫛舘山寺道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むらくしかんざんじどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冷川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひえかわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">船原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふなばら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊豆中央道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いずちゅうおうどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新掛塚橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんかけつかばし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">修善寺道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しゅぜんじどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊豆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いず</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日本平</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にほんだいら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西伊豆</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしいず</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜名湖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はまなこ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">南富士</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みなみふじ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">熱海</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あたみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富士見</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふじみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清水日本平</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しみずにほんだいら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本坂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほんざか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">音羽蒲郡有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おとわがまごおりゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小坂井</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こざかい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶臼山高原道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちゃうすやまこうげんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尾張</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おわり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小牧東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こまきひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">知多半島道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちたはんとうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">南知多道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みなみちたどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">知多半島横断道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちたはんとうおうだんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">衣浦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きぬうら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">猿投</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さなげ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三河湾</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みかわわん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鳳来寺山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほうらいじさん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本宮山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほんぐうさん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奥志摩</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おくしま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊勢二見鳥羽</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いせふたみとば</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊勢志摩</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いせしま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">飛騨美濃道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひだみのどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">乗鞍</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のりくら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中津川道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なかつがわどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長良川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながらがわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">どうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊吹山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いぶきやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">琵琶湖大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">びわこおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">近江大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おうみおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日野水口道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひのみなくちどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">途中</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とちゅう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奥比叡</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おくひえい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">比叡山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひえいざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">嵐山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あらしやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高雄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかお</t>
+  </si>
+  <si>
+    <t xml:space="preserve">京都縦貫自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きょうとじゅうかんじどうしゃどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">綾部宮津道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あやべみやづどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈良奥山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ならおくやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新若草山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんわかくさやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高円山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかまどやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">第二阪奈有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいにはんなゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">信貴生駒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しぎいこま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鳥飼仁和寺大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とりかいにわじおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">堺泉北有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さかいせんぼくゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">関西国際空港連絡橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かんさいこくさいくうこうれんらくきょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菅原城北大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すがはらしろきたおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高野龍神</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうやりゅうじん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">紀</t>
+  </si>
+  <si>
+    <t xml:space="preserve">き</t>
+  </si>
+  <si>
+    <t xml:space="preserve">川河口大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かわかこうおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">那智山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なちざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">遠阪</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とおさか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西宮北道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしのみやきたどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">六甲有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ろっこうゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">表六甲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おもてろっこう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">裏六甲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うらろっこう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">六甲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ろっこう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">六甲北有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ろっこうきたゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北神</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほくしん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新神戸</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんこうべ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西神戸有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしこうべゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在来線</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ざいらいせん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山麓</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんろく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">摩耶大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まやおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">芦有</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ろゆう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岡南大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうなんおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岡山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おかやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水玉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みずたま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">広島熊野道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひろしまくまのどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安芸灘大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あきなだおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尾道大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おのみちおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">草津沼田道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くさつぬまたどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海田大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かいたおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山口宇部有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまぐちうべゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">彦島有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひこしまゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">萩有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はぎゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津峯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つのみね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高松坂出有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかまつさかいでゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">屋島</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やしま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東予道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうよどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西海道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしうみどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高知桂浜道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうちかつらはまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浦戸大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うらどおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仁淀川河口大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">によどがわかこうおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冷水道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひやみずどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福岡前原道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふくおかまえばるどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">二丈浜玉道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にじょうはまたまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鳥栖筑紫野道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とすちくしのどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三瀬</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みつせ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">厳木多久道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きゅうらぎたくどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">国見道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くにみどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">平戸大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひらどおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">矢上大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やがみおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">川平道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かわびらどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松浦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつうら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生月大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いきつきおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西海</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さいかい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大島大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおしまおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仁多峠循環自動車道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にたとうげじゅんかんじどうしゃどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天草下島横断有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あまくさしもしまおうだんゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">阿蘇登山有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あそとざんゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">阿蘇山公園道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あそさんこうえんどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">臼杵坂</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うすきさか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">市有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いちゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大野川大橋有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおのがわおおはしゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大分湯</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおいたゆ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">平有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひらゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">米良有料道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めらゆうりょうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大分空港道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおいたくうこうどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">久住高原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くじゅうこうげん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">葉道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小倉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おぐら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">浜道路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はまどうろ</t>
   </si>
 </sst>
 </file>
@@ -31349,7 +32760,7 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -31661,6 +33072,1962 @@
       </c>
       <c r="B38" s="1" t="s">
         <v>7927</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B241"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.74"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7928</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7929</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7930</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7931</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>7932</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7933</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7934</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7935</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>7936</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7937</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>7938</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7939</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>7940</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7941</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>7942</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7943</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>7944</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7945</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>7946</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7947</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>7948</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7949</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>7950</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7951</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>7952</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7953</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>7954</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7955</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>7956</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7957</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>7958</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7959</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>7960</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7961</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>7962</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7963</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>7964</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7965</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>7966</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7967</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>7968</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7969</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>7970</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7971</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>7972</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7973</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>7974</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7975</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>7976</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7977</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>7978</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7979</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>7980</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7981</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>3300</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3301</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>7982</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7983</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>7984</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>7985</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>7986</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7987</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>7988</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7989</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>7990</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7991</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>7992</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7993</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>7994</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>7995</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>7996</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>7997</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>7998</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>7999</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>8000</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8001</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>8002</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8003</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>8004</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>8005</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>8006</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8007</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>8008</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8009</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>8010</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8011</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>8012</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8013</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>8014</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>8015</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>8016</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>8017</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>8018</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>8019</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>8020</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8021</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>8022</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>8023</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>8024</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>8025</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>3692</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>8026</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>8027</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>8028</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>8029</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>8030</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8031</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>8032</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>8033</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>8034</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8035</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>8036</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>8037</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>8038</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>8039</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>8040</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8041</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>8042</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>8043</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>8044</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>8045</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>8046</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>8047</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>8048</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>8049</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>8050</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>8051</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>8052</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>8053</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>8054</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>8055</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>8056</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>8057</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>8058</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>8059</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>8060</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>8061</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>8062</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>8063</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>8064</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>8065</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>8066</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>8067</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>8068</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>8069</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>8070</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>8071</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>8072</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>8073</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>8074</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>8075</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>8076</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>8077</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>8078</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>8079</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>8080</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>8081</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>8082</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>8083</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>8084</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>8085</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>8086</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>8087</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>8088</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>8089</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>8090</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>8091</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>8092</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>8093</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>8094</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>2595</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>8095</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>8096</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>8097</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>8098</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>8099</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>8101</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>8102</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>8103</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>8104</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>8105</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>8106</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>5627</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>8107</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>8108</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>8109</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>8110</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>8111</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>8112</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>8113</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>8114</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>8115</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>8116</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>8117</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>8118</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>8119</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>8120</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>8121</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>8122</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>8123</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>8124</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>8125</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>8126</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>8127</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>8128</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>8129</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>8130</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>8131</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>8132</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>8133</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>8134</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>8135</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>8136</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>8137</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>8138</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>8139</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>8140</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>8141</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>8142</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>8143</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>8144</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>8145</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>8146</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>8147</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>8148</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>8149</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>8150</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>8151</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>8152</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>8153</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>8154</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>8155</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>8156</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>8157</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>8158</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>8159</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>8160</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>8161</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>8162</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>8163</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>8164</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>8165</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>8166</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>8167</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>8168</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>8169</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>8170</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>8171</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>8172</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>8173</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>8174</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>8175</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>8176</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>8177</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>8178</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>8179</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>8180</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>8181</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>8182</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>8183</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>8184</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>8185</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>8186</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>8187</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>8188</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>8189</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>8191</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>8193</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>8194</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>8195</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>8196</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>8197</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>8198</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>8199</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>8201</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>8202</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>8203</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>8204</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>8205</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>8206</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>8207</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>8208</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>8209</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>8210</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>8211</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>8212</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>8213</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>8214</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>8215</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>8216</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>8217</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>8218</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>8219</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>8220</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>8221</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>8222</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>8223</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>8224</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>8225</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>8226</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>8227</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>8228</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>8229</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>8230</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>8231</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>8232</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>8233</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>8234</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>8235</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>8236</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>8237</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>8238</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>8239</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>8240</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>8241</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>8242</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>8243</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>8244</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
+        <v>8245</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>8246</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>8247</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>8248</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>8249</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>8250</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>8251</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>8252</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="s">
+        <v>8253</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>8254</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
+        <v>8255</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>8256</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
+        <v>8257</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>8258</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>8259</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>8260</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>8261</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>8262</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>8263</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>8264</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>8265</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>8266</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>8267</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>8268</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>8269</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>8270</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>8271</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>8272</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>8273</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>8274</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>8275</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>8276</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
+        <v>8277</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>8278</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>8279</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>8280</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>8281</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>8282</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>8283</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>8284</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>8285</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>8286</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>8287</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>8288</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>8289</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>8290</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>8291</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>8292</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>8293</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>8294</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>8295</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>8296</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>8297</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>8298</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>8299</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>8301</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>8302</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="s">
+        <v>8303</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>8304</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
+        <v>8305</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>8306</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
+        <v>8307</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>8308</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
+        <v>8309</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>8310</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>8311</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>8312</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="s">
+        <v>8313</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>8314</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
+        <v>8315</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>8316</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>8317</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>8318</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
+        <v>8319</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>2278</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>8320</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>8321</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
+        <v>8322</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>8323</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>8324</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>8325</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>8326</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>8327</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
+        <v>8328</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>8329</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>8330</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>8331</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>8332</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>8333</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>8334</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>8335</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>8336</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>8337</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>8338</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>8339</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>8340</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>8341</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>8342</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>8343</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>8344</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>8345</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>8346</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>8347</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>8348</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>8349</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>8350</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>8351</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>8352</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>8353</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>8354</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>8355</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>8356</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>8357</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>8358</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>8359</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
+        <v>8360</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>8361</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
+        <v>8362</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>8363</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
+        <v>8364</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>8365</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="1" t="s">
+        <v>8366</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>8367</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
+        <v>8368</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>8369</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
+        <v>8370</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>8371</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="1" t="s">
+        <v>8372</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>8373</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="1" t="s">
+        <v>8374</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>8375</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="1" t="s">
+        <v>8376</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>8377</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="1" t="s">
+        <v>8378</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>8379</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="1" t="s">
+        <v>8380</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>8381</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="1" t="s">
+        <v>8382</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>8383</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="1" t="s">
+        <v>8384</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>8385</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>8386</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>8387</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
+        <v>8388</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>8389</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="1" t="s">
+        <v>8390</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>8391</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
+        <v>8392</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>8393</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="1" t="s">
+        <v>8394</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>8395</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
+        <v>8396</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>8397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "TennoYomikata" sheet in "OtoYakuNoHeyaYomikataJiten.xlsx" file Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenTennoYomikataJitenMultimapFactoryBean.sheetName" property in "configuration.properties" Extends "org.springframework.beans.factory.StringMultiMapFromResourceFactoryBean" class by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenTennoYomikataJitenMultimapFactoryBean" Class Update "applicationContext.xml" Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenTennoYomikataJitenMultimapFactoryBean.getObject()" method
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -20,6 +20,7 @@
     <sheet name="MintetsuYomikataJiten" sheetId="10" state="visible" r:id="rId12"/>
     <sheet name="SintomeiYomikataJiten" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="YuryodoYomikataJiten" sheetId="12" state="visible" r:id="rId14"/>
+    <sheet name="TennoYomikata" sheetId="13" state="visible" r:id="rId15"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8984" uniqueCount="8398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9440" uniqueCount="8852">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -26576,6 +26577,1368 @@
   </si>
   <si>
     <t xml:space="preserve">はまどうろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">神武天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じんむてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">畝傍山東北陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うねびやまのうしとらのすみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">綏靖天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すいぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桃花鳥田丘上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つきだのおかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安寧天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あんねいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">畝傍山西南御陰井上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うねびやまのひつじさるのみほどのいのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">畝傍山南纖沙溪上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うねびやまのみなみのまなごのたにのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝昭天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうしょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">掖上博多山上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わきのかみのはかたのやまのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝安天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうあんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">玉手丘上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たまてのおかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝霊天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうれいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">片丘馬坂陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かたおかのうまさかのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝元天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうげんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">剣池嶋上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つるぎのいけのしまのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">開化天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かいかてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">春日率川坂上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かすがのいざかわのさかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">崇神天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すじんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山邊道勾岡上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまのべのみちのまがりのおかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">垂仁天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すいにんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菅原伏見東陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すがわらのふしみのひがしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">景行天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">けいこうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山邊道上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまのべのみちのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">成務天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せいむてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">狹城盾列池後陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さきのたたなみのいけじりのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仲哀天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちゅうあいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">惠我長野西陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えがのながののにしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">応神天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おうじんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">惠我藻伏崗陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えがのもふしのおかのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仁徳天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にんとくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">百舌鳥耳原中陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もずのみみはらのなかのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">履中天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">りちゅうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">百舌鳥耳原南陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もずのみみはらのみなみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">反正天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はんぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">百舌鳥耳原北陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もずのみみはらのきたのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">允恭天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いんぎょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">惠我長野北陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えがのながののきたのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安康天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あんこうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菅原伏見西陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すがわらのふしみのにしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">雄略天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆうりゃくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">丹比高鷲原陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たじひのたかわしのはらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清寧天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せいねいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河内坂門原陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうちのさかどのはらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">顕宗天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">けんぞうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">傍丘磐坏丘南陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かたおかのいわつきのおかのみなみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仁賢天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にんけんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">埴生坂本陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はにゅうのさかもとのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武烈天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ぶれつてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">傍丘磐坏丘北陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かたおかのいわつきのおかのきたのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">継体天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">けいたいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三嶋藍野陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みしまのあいののみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安閑天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あんかんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">古市高屋丘陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふるちのたかやのおかのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宣化天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せんかてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">身狹桃花鳥坂上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むさのつきさかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">欽明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きんめいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">檜隈坂合陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひのくまのさかあいのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">敏達天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">びだつてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河内磯長中尾陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうちのしながのなかのおのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">用明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ようめいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">河内磯長原陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうちのしながのはらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">崇峻天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すしゅんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">倉梯岡陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くらはしのおかのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">推古天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すいこてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">磯長山田陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しながのやまだのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">舒明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じょめいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">押坂内陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おさかのうちのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">皇極天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうぎょくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">越智崗上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おちのおかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝徳天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうとくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大阪磯長陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおさかのしながのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斉明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さいめいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天智天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">てんじてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山科陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やましなのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">弘文天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうぶんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長等山前陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながらのやまさきのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天武天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">てんむてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">檜隈大内陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひのくまのおおうちのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">持統天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じとうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">文武天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もんむてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">檜隈安古岡上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひのくまのあこのおかのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">元明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">げんめいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈保山東陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なほやまのひがしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">元正天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">げんしょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈保山西陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なほやまのにしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">聖武天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しょうむてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">佐保山南陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さほやまのみなみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝謙天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうけんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高野陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかののみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淳仁天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じゅんにんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淡路陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あわじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">称徳天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しょうとくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">光仁天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうにんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田原東陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たはらのひがしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桓武天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かんむてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">柏原陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かしわばらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">平城天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">へいぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">楊梅陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまもものみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">嵯峨天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さがてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">嵯峨山上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さがのやまのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">淳和天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じゅんなてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大原野西嶺上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおはらののにしのみねのえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仁明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にんみょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深草陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふかくさのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">文徳天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もんとくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">田邑陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たむらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清和天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せいわてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水尾山陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みずのおやまのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">陽成天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ようぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">神楽岡東陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かぐらがおかのひがしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">光孝天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうこうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後田邑陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのたむらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宇多天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うだてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大内山陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおうちやまのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">醍醐天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいごてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後山科陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのやましなのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">朱雀天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すざくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">醍醐陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいごのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">村上天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むらかみてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">村上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むらかみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冷泉天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">れいぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桜本陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さくらもとのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">円融天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えんゆうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後村上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのむらかみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">花山天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かざんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">紙屋川上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かみやがわのほとりのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">一条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いちじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">圓融寺北陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えんゆうじのきたのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北山陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたやまのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後一条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごいちじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菩提樹院陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ぼだいじゅいんのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後朱雀天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごすざくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">圓乘寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えんじょうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後冷泉天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごれいぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">圓教寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えんきょうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後三条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごさんじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">圓宗寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えんそうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白河天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しらかわてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">成菩提院陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じょうぼだいいんのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">堀河天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほりかわてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後圓教寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのえんきょうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">鳥羽天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とばてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安楽壽院陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あんらくじゅいんのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">崇徳天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すとくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白峯陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しらみねのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">近衞天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">このえてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">安樂壽院南陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あんらくじゅいんのみなみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後白河天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごしらかわてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">法住寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ほうじゅうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">二条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香隆寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうりゅうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">六条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ろくじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">清閑寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">せいかんじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">高倉天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たかくらてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後清閑寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのせいかんじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">阿彌陀寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あみだじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後鳥羽天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごとばてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大原陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおはらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">土御門天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つちみかどてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金原陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かねがはらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">順徳天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じゅんとくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仲恭天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちゅうきょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">九條陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くじょうのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後堀河天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごほりかわてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">觀音寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かんおんじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">四条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">月輪陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つきのわのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後嵯峨天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごさがてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">嵯峨南陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さがのみなみのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後深草天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごふかくさてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深草北陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふかくさのきたのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">亀山天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かめやまてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">龜山陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かめやまのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後宇多天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごうだてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蓮華峯寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">れんげぶじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伏見天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふしみてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後伏見天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごふしみてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後二条天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごにじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北白河陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたしらかわのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">花園天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はなぞのてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">十楽院上陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">じゅうらくいんのうえのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後醍醐天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごだいごてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">塔尾陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうのおのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山国陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やまくにのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">光明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうみょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大光明寺陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいこうみょうじのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">崇光天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すこうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後円融天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごえんゆうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後村上天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごむらかみてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">檜尾陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひのおのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長慶天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちょうけいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">嵯峨東陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さがのひがしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後亀山天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごかめやまてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">嵯峨小倉陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さがのおぐらのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後小松天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごこまつてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">称光天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しょうこうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後花園天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごはなぞのてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後山国陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのやまくにのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後土御門天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごつちみかどてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後柏原天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごかしわばらてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後奈良天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごならてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">正親町天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおぎまちてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後陽成天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごようぜいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後水尾天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごみずのおてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">明正天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めいしょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後光明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごこうみょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後西天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごさいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">霊元天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">れいげんてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東山天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひがしやまてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">中御門天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なかみかどてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桜町天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さくらまちてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">桃園天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ももぞのてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後桜町天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごさくらまちてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後桃園天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごももぞのてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">光格天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうかくてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後月輪陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのつきのわのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">仁孝天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にんこうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">孝明天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こうめいてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">後月輪東山陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のちのつきのわのひがしのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">明治天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めいじてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伏見桃山陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふしみのももやまのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大正天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たいしょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">多摩陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たまのみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">昭和天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しょうわてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">武藏野陵</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むさしののみささぎ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">今上天皇</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きんじょうてんのう</t>
   </si>
 </sst>
 </file>
@@ -33092,7 +34455,7 @@
   </sheetPr>
   <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -35028,6 +36391,1858 @@
       </c>
       <c r="B241" s="1" t="s">
         <v>8397</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B228"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.97"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>8398</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8399</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8400</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8401</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8402</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8403</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8404</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8405</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8406</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8407</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>8408</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8409</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>8410</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8411</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>8412</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8413</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>8414</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8415</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>8416</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8417</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>8418</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8419</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>8420</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8421</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>8422</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8423</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>8424</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8425</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>8426</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8427</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>8428</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8429</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>8430</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8431</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>8432</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8433</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>8434</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8435</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>8436</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8437</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>8438</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8439</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>8440</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8441</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>8442</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8443</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>8444</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8445</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>8446</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8447</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>8448</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8449</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>8450</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8451</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>8452</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8453</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>8454</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8455</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>8456</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8457</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>8458</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8459</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>8460</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8461</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>8462</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8463</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>8464</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8465</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>8466</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8467</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>8468</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8469</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>8470</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8471</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>8472</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8473</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>8474</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8475</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>8476</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>8477</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>8478</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8479</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>8480</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8481</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>8482</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8483</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>8484</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8485</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>8486</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>8487</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>8488</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>8489</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>8490</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>8491</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>8492</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8493</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>8494</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>8495</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>8496</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>8497</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>8498</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>8499</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>8500</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>8501</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>8502</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>8503</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>8504</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8505</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>8506</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>8507</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>8508</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8509</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>8510</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>8511</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>8512</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>8513</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>8514</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8515</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>8516</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>8517</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>8518</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>8519</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>8520</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>8521</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>8522</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>8523</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>8524</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>8525</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>8526</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>8527</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>8528</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>8529</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>8530</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>8531</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>8532</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>8533</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>8534</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>8535</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>8536</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>8537</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>8538</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>8539</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>8540</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>8541</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>8542</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>8543</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>8544</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>8545</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>8546</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>8547</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>8548</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>8549</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>8550</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>8551</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>8552</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>8553</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>8554</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>8555</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>8556</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>8557</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>8558</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>8559</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>8560</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>8561</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>8562</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>8563</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>8564</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>8565</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>8566</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>8567</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>8568</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>8569</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>8570</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>8571</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>8572</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>8573</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>8574</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>8575</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>8576</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>8577</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>8578</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>8579</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>8580</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>8581</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>8582</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>8583</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>8584</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>8585</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>8586</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>8587</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>8588</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>8589</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>8590</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>8591</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>8592</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>8593</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>8594</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>8595</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>8596</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>8597</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>8598</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>8600</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>8601</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>8602</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>8603</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>8604</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>8605</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>8606</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>8607</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>8608</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>8609</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>8610</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>8611</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>8612</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>8613</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>8614</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>8615</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>8616</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>8617</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>8618</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>8619</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="s">
+        <v>8620</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>8621</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>8622</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>8623</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>8624</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>8625</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="s">
+        <v>8626</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>8627</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
+        <v>8628</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>8629</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>8630</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>8631</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="s">
+        <v>8632</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>8633</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>8634</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>8635</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>8636</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>8637</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>8638</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>8639</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
+        <v>8640</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>8641</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
+        <v>8642</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>8643</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="s">
+        <v>8644</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>8645</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>8646</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>8647</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>8648</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>8649</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="s">
+        <v>8650</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>8651</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="s">
+        <v>8652</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>8653</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="s">
+        <v>8654</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>8655</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="s">
+        <v>8656</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>8657</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>8658</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>8659</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>8660</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>8661</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>8662</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>8663</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>8664</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>8665</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="s">
+        <v>8666</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>8667</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>8668</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>8669</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>8670</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>8671</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>8672</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>8673</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>8674</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>8675</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>8676</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>8677</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>8678</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>8679</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>8680</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>8681</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>8682</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>8683</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>8684</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>8685</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>8686</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>8687</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>8688</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>8689</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>8690</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>8691</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>8692</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>8693</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>8694</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>8695</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>8696</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>8697</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>8698</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>8699</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>8700</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>8701</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>8702</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>8703</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>8704</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>8705</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>8706</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>8707</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>8708</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>8709</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>8710</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>8711</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>8712</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>8713</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>8714</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>8715</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>8716</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>8717</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>8718</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>8719</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>8720</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>8721</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
+        <v>8722</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>8723</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>8724</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>8725</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>8726</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>8727</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>8728</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>8729</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="s">
+        <v>8730</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>8731</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
+        <v>8732</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>8733</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
+        <v>8734</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>8735</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>8736</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>8737</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>8738</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>8739</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>8740</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>8741</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>8742</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>8743</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>8744</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>8745</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>8746</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>8747</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>8748</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>8749</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>8750</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>8751</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>8752</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>8753</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
+        <v>8754</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>8755</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>8756</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>8757</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
+        <v>8758</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>8759</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>8760</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>8761</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>8762</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>8763</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>8764</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>8765</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>8766</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>8767</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>8768</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>8769</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>8770</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>8771</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>8772</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>8773</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>8774</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>8775</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>8776</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>8777</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>8778</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>8779</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>8780</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>8781</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="s">
+        <v>8782</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>8783</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
+        <v>8784</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>8785</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
+        <v>8786</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>8787</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
+        <v>8788</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>8789</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>8790</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>8791</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="s">
+        <v>8792</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>8793</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
+        <v>8794</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>8795</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>8796</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>8797</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
+        <v>8798</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>8799</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>8800</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>8801</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
+        <v>8802</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>8803</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>8804</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>8805</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>8806</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>8807</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
+        <v>8808</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>8809</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>8810</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>8811</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>8812</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>8813</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>8814</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>8815</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>8816</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>8817</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>8818</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>8819</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>8820</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>8821</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>8822</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>8823</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>8824</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>8825</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>8826</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>8827</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>8828</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>8829</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>8830</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>8831</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>8832</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>8833</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>8834</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>8835</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>8836</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>8837</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>8838</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>8839</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
+        <v>8840</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>8841</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
+        <v>8842</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>8843</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
+        <v>8844</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>8845</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="1" t="s">
+        <v>8846</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>8847</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
+        <v>8848</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>8849</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
+        <v>8850</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>8851</v>
       </c>
     </row>
   </sheetData>
@@ -35084,8 +38299,8 @@
   </sheetPr>
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Add "FukuokaKousokuDouroYomikata" sheet in "src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx" file Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenFukuokaKousokuDouroYomikataJitenMultimapFactoryBean.sheetName" property in "configuration.properties" Extend "org.springframework.beans.factory.StringMultiMapFromResourceFactoryBean" class by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenFukuokaKousokuDouroYomikataJitenMultimapFactoryBean" class Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenFukuokaKousokuDouroYomikataJitenMultimapFactoryBean.getObject()" method Update "src/main/resources/applicationContext.xml" file
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,6 +21,7 @@
     <sheet name="SintomeiYomikataJiten" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="YuryodoYomikataJiten" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="TennoYomikata" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="FukuokaKousokuDouroYomikata" sheetId="14" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9440" uniqueCount="8852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9592" uniqueCount="8998">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -27939,6 +27940,444 @@
   </si>
   <si>
     <t xml:space="preserve">きんじょうてんのう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香椎東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かしいひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香住ヶ丘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かすみがおか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香椎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かしい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">香椎浜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かしいはま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">名島</t>
+  </si>
+  <si>
+    <t xml:space="preserve">なじま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">貝塚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かいづか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">箱崎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はこざき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東浜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひがしはま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千鳥橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちどりばし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">築港</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちっこう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">天神北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">てんじんきた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西公園</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしこうえん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">百道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ももち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">愛宕</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あたご</t>
+  </si>
+  <si>
+    <t xml:space="preserve">姪浜</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めいのはま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石丸</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いしまる</t>
+  </si>
+  <si>
+    <t xml:space="preserve">福重</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふくしげ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千代</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちよ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">呉服町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ごふくまち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">博多駅東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はかたえきひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">豊</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆたか</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東光</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とうこう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">榎田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えのきだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">半道橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はんみちばし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">月隈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つきぐま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">隈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大野城</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおのじょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水城</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みずき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">太宰府</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だざいふ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">空港通</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くうこうどおり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">松島</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まつしま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">多</t>
+  </si>
+  <si>
+    <t xml:space="preserve">た</t>
+  </si>
+  <si>
+    <t xml:space="preserve">津</t>
+  </si>
+  <si>
+    <t xml:space="preserve">つ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">粕屋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かすや</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長野</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ながの</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小倉南区</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こくらみなみく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">横代</t>
+  </si>
+  <si>
+    <t xml:space="preserve">よこしろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">若園</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わかぞの</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北方</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたがた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">篠崎南</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しのざきみなみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">紫川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むらさきがわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">篠崎北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しのざききた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大手町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおてまち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">勝山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かつやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小倉北区</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こくらきたく</t>
+  </si>
+  <si>
+    <t xml:space="preserve">菜園場</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さえんば</t>
+  </si>
+  <si>
+    <t xml:space="preserve">下到津</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しもいとうづ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小倉駅北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こくらえききた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">許斐町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">このみまち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">東港</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひがしみなと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日明</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひあがり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西港</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしみなと</t>
+  </si>
+  <si>
+    <t xml:space="preserve">戸畑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とばた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">若戸大橋</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わかとおおはし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大字戸畑</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とばたくとばた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門司</t>
+  </si>
+  <si>
+    <t xml:space="preserve">春日</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かすが</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大里</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だいり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富野</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とみの</t>
+  </si>
+  <si>
+    <t xml:space="preserve">足立</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あだち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山路</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さんじ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大谷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおたに</t>
+  </si>
+  <si>
+    <t xml:space="preserve">黒崎</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くろさき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小嶺</t>
+  </si>
+  <si>
+    <t xml:space="preserve">こみね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">馬場山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ばばやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">八幡区西区茶屋の原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">やはたにしくちゃやのはる</t>
+  </si>
+  <si>
+    <t xml:space="preserve">枝光</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えだみつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大字枝光</t>
+  </si>
+  <si>
+    <t xml:space="preserve">神山町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かみやままち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">糟屋郡粕屋町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かすやぐんかすやまち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">戸原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とばら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">蒲田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かまた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">西月隈</t>
+  </si>
+  <si>
+    <t xml:space="preserve">にしつきぐま</t>
   </si>
 </sst>
 </file>
@@ -36411,8 +36850,8 @@
   </sheetPr>
   <dimension ref="A1:B228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38243,6 +38682,641 @@
       </c>
       <c r="B228" s="1" t="s">
         <v>8851</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B76"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.27"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>8852</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>8853</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8854</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8855</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8856</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8857</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8858</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8859</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8860</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>8861</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>8862</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>8863</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>8864</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8865</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8866</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>8867</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>8868</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>8869</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>8870</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>8871</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>8872</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>8873</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>8874</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>8875</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>8876</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>8877</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>8878</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>8879</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>8880</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>8881</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>8882</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>8883</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>8884</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>8885</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>8340</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>8341</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>8886</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>8887</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>8888</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>8889</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>8890</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>8891</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>8892</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>8893</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>8894</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>8895</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>8896</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>8897</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>8898</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>8899</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>8900</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>8901</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>8902</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>8903</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>8904</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>8905</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>8906</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>8907</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>8908</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>8909</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>8910</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>8911</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>8912</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>8913</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>8914</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>8915</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>8916</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>8917</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>8918</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>8919</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>8920</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>8921</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>8922</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>8923</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>8924</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>8925</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>8926</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>8927</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>8928</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>8929</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>8930</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>8931</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>8932</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>8933</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>8934</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>8935</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>8936</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>8937</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>8938</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>8939</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>8940</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>8941</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>8942</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>8943</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>8944</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>8945</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>8946</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>8947</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>8948</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>8949</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>8950</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>8951</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>8952</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>8953</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>8954</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>8955</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>8956</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>8957</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>8958</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>8959</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>8960</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>8961</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>8962</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>8963</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>8964</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>8965</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>8966</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>8967</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>8968</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>8969</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>8970</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>8971</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>8972</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>8973</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>8974</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>8975</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>8976</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>8977</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>8978</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>8979</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>8980</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>8981</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>8982</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>8983</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>8984</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>8985</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>8986</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>8987</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>8986</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>8988</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>8989</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>8990</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>8991</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>8992</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>8993</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>8994</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>8995</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>8996</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>8997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add "ZenkokuKousokuDouroYomikata" sheet in "src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx" file Add "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenZenkokuKousokuDouroYomikataJitenMultimapFactoryBean.sheetName" property in "src/main/resources/configuration.properties" file Extend "org.springframework.beans.factory.StringMultiMapFromResourceFactoryBean" class by "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenZenkokuKousokuDouroYomikataJitenMultimapFactoryBean" class Update "org.springframework.beans.factory.OtoYakuNoHeyaYomikataJitenZenkokuKousokuDouroYomikataJitenMultimapFactoryBean.getObject()" method Update "src/main/resources/applicationContext.xml" file
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,6 +22,7 @@
     <sheet name="YuryodoYomikataJiten" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="TennoYomikata" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="FukuokaKousokuDouroYomikata" sheetId="14" state="visible" r:id="rId16"/>
+    <sheet name="ZenkokuKousokuDouroYomikata" sheetId="15" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9592" uniqueCount="8998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9722" uniqueCount="9126">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -28378,6 +28379,390 @@
   </si>
   <si>
     <t xml:space="preserve">にしつきぐま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">国縫</t>
+  </si>
+  <si>
+    <t xml:space="preserve">くんぬい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">長万部</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おしゃまんべ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">静狩</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しずかり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">豊浦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とようら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">豊浦噴火湾</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とようらふんかわん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">虻田洞爺湖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あぶたとうやこ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伊達</t>
+  </si>
+  <si>
+    <t xml:space="preserve">だて</t>
+  </si>
+  <si>
+    <t xml:space="preserve">有珠山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">うすざん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">室蘭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">むろらん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">本輪西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">もとわにし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">登別室蘭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のぼりべつむろらん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">富浦</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とみうら</t>
+  </si>
+  <si>
+    <t xml:space="preserve">登別東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のぼりべつひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">萩野</t>
+  </si>
+  <si>
+    <t xml:space="preserve">はぎの</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白老</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しらおい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">樽前</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たるまえ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">苫小牧西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とまこまいにし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">苫小牧東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とまこまいひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">美沢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みさわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千歳</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちとせ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千歳恵庭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちとせえにわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">恵庭</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えにわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">輪厚</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わっつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北広島</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたひろしま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札幌南</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっぽろみなみ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大谷地</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おおやち</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北郷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">きたごう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札幌</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっぽろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">江別西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えべつにし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">野幌</t>
+  </si>
+  <si>
+    <t xml:space="preserve">のっぽろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">江別東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">えべつひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">岩見沢</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いわみざわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">三笠</t>
+  </si>
+  <si>
+    <t xml:space="preserve">みかさ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">美唄</t>
+  </si>
+  <si>
+    <t xml:space="preserve">びばい</t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶志内</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちゃしない</t>
+  </si>
+  <si>
+    <t xml:space="preserve">奈井江砂川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ないえすながわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">砂川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">すながわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">滝川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">たきかわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふかがわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">音江</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おとえ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">旭川鷹栖</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あさひかわたかす</t>
+  </si>
+  <si>
+    <t xml:space="preserve">旭川北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あさひかわきた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">比布大雪</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ひっぷだいせつ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">和寒</t>
+  </si>
+  <si>
+    <t xml:space="preserve">わさむ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札樽道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっそんどう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小樽</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おたる</t>
+  </si>
+  <si>
+    <t xml:space="preserve">朝里</t>
+  </si>
+  <si>
+    <t xml:space="preserve">あさり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">銭函</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ぜにばこ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金山</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かなやま</t>
+  </si>
+  <si>
+    <t xml:space="preserve">手稲</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ていね</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札幌西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっぽろにし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">新川</t>
+  </si>
+  <si>
+    <t xml:space="preserve">しんかわ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札幌北</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっぽろきた</t>
+  </si>
+  <si>
+    <t xml:space="preserve">伏古</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふしこ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">雁来</t>
+  </si>
+  <si>
+    <t xml:space="preserve">かりき</t>
+  </si>
+  <si>
+    <t xml:space="preserve">千歳東</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ちとせひがし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">追分町</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おいわけちょう</t>
+  </si>
+  <si>
+    <t xml:space="preserve">夕張</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ゆうばり</t>
+  </si>
+  <si>
+    <t xml:space="preserve">十勝清水</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とかちしみず</t>
+  </si>
+  <si>
+    <t xml:space="preserve">十勝平原</t>
+  </si>
+  <si>
+    <t xml:space="preserve">とかちへいげん</t>
+  </si>
+  <si>
+    <t xml:space="preserve">芽室</t>
+  </si>
+  <si>
+    <t xml:space="preserve">めむろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">音更帯広</t>
+  </si>
+  <si>
+    <t xml:space="preserve">おとふけおびひろ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">池田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">いけだ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">深川西</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ふかがわにし</t>
   </si>
 </sst>
 </file>
@@ -38702,13 +39087,13 @@
   </sheetPr>
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -38720,603 +39105,1151 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>8852</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8853</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8854</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8855</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8856</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8857</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8858</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8859</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8860</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8861</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>8862</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8863</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>8864</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8865</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>8866</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>8867</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>8868</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8869</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>8870</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8871</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>8872</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8873</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>8874</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8875</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>8876</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8877</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>8878</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8879</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>8880</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8881</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>8882</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8883</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>8884</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8885</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>8340</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8341</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>8886</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8887</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>8888</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8889</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>8890</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8891</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>8892</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8893</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>8894</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>8895</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>8896</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>8897</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>8898</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8899</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>8900</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8901</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>8902</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8903</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>8904</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8905</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>8906</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8907</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>8908</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8909</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>8910</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8911</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>8912</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8913</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>8914</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8915</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>8916</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8917</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>8918</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8919</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>8920</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8921</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>8922</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8923</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>8924</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8925</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>8926</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8927</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>8928</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>8929</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>8930</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>8931</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>8932</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>8933</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>8934</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8935</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>8936</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8937</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>8938</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>8939</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>8940</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>8941</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>8942</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>8943</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>8944</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>8945</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>8946</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>8947</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>8948</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>8949</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>8950</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>8951</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>8952</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>8953</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>8954</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>8955</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>8956</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8957</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>8958</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>8959</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>8960</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8961</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>8962</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>8963</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>8964</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>2674</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>8965</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8966</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>8967</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>8968</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>8969</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>8970</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>8971</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>8972</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>8973</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>8974</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>8975</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>8976</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>8977</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>8978</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>8979</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>8980</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>8981</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>8982</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>8983</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>8984</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>8985</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>8986</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>8987</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>8986</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>8988</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>8989</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>8990</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>8991</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>8992</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>8993</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>8994</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>8995</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>8996</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>8997</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B65"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.85"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8852</v>
+        <v>8998</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8853</v>
+        <v>8999</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8854</v>
+        <v>9000</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8855</v>
+        <v>9001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8856</v>
+        <v>9002</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8857</v>
+        <v>9003</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8858</v>
+        <v>9004</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8859</v>
+        <v>9005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8860</v>
+        <v>9006</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>8861</v>
+        <v>9007</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8862</v>
+        <v>9008</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>8863</v>
+        <v>9009</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>8864</v>
+        <v>9010</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>8865</v>
+        <v>9011</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8866</v>
+        <v>9012</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>8867</v>
+        <v>9013</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>8868</v>
+        <v>9014</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>8869</v>
+        <v>9015</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>8870</v>
+        <v>9016</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>8871</v>
+        <v>9017</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>8872</v>
+        <v>9018</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>8873</v>
+        <v>9019</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>8874</v>
+        <v>9020</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>8875</v>
+        <v>9021</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>8876</v>
+        <v>9022</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>8877</v>
+        <v>9023</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>8878</v>
+        <v>9024</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>8879</v>
+        <v>9025</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>8880</v>
+        <v>9026</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>8881</v>
+        <v>9027</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>8882</v>
+        <v>9028</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>8883</v>
+        <v>9029</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>8884</v>
+        <v>9030</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>8885</v>
+        <v>9031</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>8340</v>
+        <v>9032</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>8341</v>
+        <v>9033</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>8886</v>
+        <v>9034</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>8887</v>
+        <v>9035</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>8888</v>
+        <v>9036</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>8889</v>
+        <v>9037</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>8890</v>
+        <v>9038</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>8891</v>
+        <v>9039</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>8892</v>
+        <v>9040</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>8893</v>
+        <v>9041</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>8894</v>
+        <v>9042</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>8895</v>
+        <v>9043</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>8896</v>
+        <v>9044</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>8897</v>
+        <v>9045</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>8898</v>
+        <v>9046</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>8899</v>
+        <v>9047</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>8900</v>
+        <v>9048</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>8901</v>
+        <v>9049</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>8902</v>
+        <v>9050</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>8903</v>
+        <v>9051</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>8904</v>
+        <v>9052</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>8905</v>
+        <v>9053</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>8906</v>
+        <v>9054</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>8907</v>
+        <v>9055</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>8908</v>
+        <v>9056</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>8909</v>
+        <v>9057</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>8910</v>
+        <v>9058</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>8911</v>
+        <v>9059</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>8912</v>
+        <v>9060</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>8913</v>
+        <v>9061</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>8914</v>
+        <v>9062</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>8915</v>
+        <v>9063</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>8916</v>
+        <v>9064</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>8917</v>
+        <v>9065</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>8918</v>
+        <v>9066</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>8919</v>
+        <v>9067</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>8920</v>
+        <v>9068</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>8921</v>
+        <v>9069</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>8922</v>
+        <v>9070</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>8923</v>
+        <v>9071</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>8924</v>
+        <v>9072</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>8925</v>
+        <v>9073</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>8926</v>
+        <v>9074</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>8927</v>
+        <v>9075</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>8928</v>
+        <v>9076</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>8929</v>
+        <v>9077</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>8930</v>
+        <v>9078</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>8931</v>
+        <v>9079</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>8932</v>
+        <v>9080</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>8933</v>
+        <v>9081</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>8934</v>
+        <v>9082</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>8935</v>
+        <v>9083</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>8936</v>
+        <v>9084</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>8937</v>
+        <v>9085</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>8938</v>
+        <v>9086</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>8939</v>
+        <v>9087</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>8940</v>
+        <v>9088</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>8941</v>
+        <v>9089</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>8942</v>
+        <v>9090</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>8943</v>
+        <v>9091</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>8944</v>
+        <v>9092</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>8945</v>
+        <v>9093</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>8946</v>
+        <v>9094</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>8947</v>
+        <v>9095</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>8948</v>
+        <v>9096</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>8949</v>
+        <v>9097</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>8950</v>
+        <v>9098</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>8951</v>
+        <v>9099</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>8952</v>
+        <v>9100</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>8953</v>
+        <v>9101</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>8954</v>
+        <v>9102</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>8955</v>
+        <v>9103</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>8956</v>
+        <v>9104</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>8957</v>
+        <v>9105</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>8958</v>
+        <v>9106</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>8959</v>
+        <v>9107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>8960</v>
+        <v>9108</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>8961</v>
+        <v>9109</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>8962</v>
+        <v>9110</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>8963</v>
+        <v>9111</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>8964</v>
+        <v>9112</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>2674</v>
+        <v>9113</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>8965</v>
+        <v>9114</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>8966</v>
+        <v>9115</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>8967</v>
+        <v>9116</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>8968</v>
+        <v>9117</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>8969</v>
+        <v>9118</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>8970</v>
+        <v>9119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>8971</v>
+        <v>9120</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>8972</v>
+        <v>9121</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>8973</v>
+        <v>9122</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>8974</v>
+        <v>9123</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>8975</v>
+        <v>9124</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>8976</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>8977</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>8978</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>8979</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>8980</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>8981</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>8982</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>8983</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>8984</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>8985</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>8986</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>8987</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>8986</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>8988</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>8989</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>8990</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>8991</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>8992</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>8993</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>8994</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>8995</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>8996</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>8997</v>
+        <v>9125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update "ZenkokuKousokuDouroYomikata" sheet in "src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx" file
</commit_message>
<xml_diff>
--- a/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
+++ b/src/main/resources/OtoYakuNoHeyaYomikataJiten.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9722" uniqueCount="9126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9724" uniqueCount="9128">
   <si>
     <t xml:space="preserve">Page</t>
   </si>
@@ -28763,6 +28763,12 @@
   </si>
   <si>
     <t xml:space="preserve">ふかがわにし</t>
+  </si>
+  <si>
+    <t xml:space="preserve">札樽自動車道</t>
+  </si>
+  <si>
+    <t xml:space="preserve">さっそんじどうしゃどう</t>
   </si>
 </sst>
 </file>
@@ -28996,7 +29002,7 @@
   <dimension ref="A1:B199"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A2:B66 B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30616,7 +30622,7 @@
   <dimension ref="A1:B538"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="2" sqref="A2:B66 B66 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34948,7 +34954,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B66 B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -35280,7 +35286,7 @@
   <dimension ref="A1:B241"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:B66 B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37236,7 +37242,7 @@
   <dimension ref="A1:B228"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="A2:B66 B66 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39088,7 +39094,7 @@
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="A2:B66 B66 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39720,16 +39726,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B66" activeCellId="0" sqref="A2:B66 B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -39741,515 +39747,523 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8998</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8999</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9000</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9002</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>9003</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>9004</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>9006</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>9007</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9008</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>9009</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>9010</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>9011</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>9012</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>9013</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>9014</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>9015</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>9016</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>9017</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>9018</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>9019</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>9020</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>9021</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>9022</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>9023</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>9024</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>9025</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>9026</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>9027</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>9028</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>9029</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>9030</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>9031</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>9032</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>9033</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>9034</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>9035</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>9036</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>9037</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>9038</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>9039</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>9040</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>9041</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>9042</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>9043</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>9044</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>9045</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>9046</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>9047</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>9048</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>9049</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>9050</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>9051</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>9052</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>9053</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>9054</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>9055</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>9056</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>9057</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>9058</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>9059</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>9060</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>9061</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>9062</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>9063</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>9064</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>9065</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>9066</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>9067</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>9068</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>9069</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>9070</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>9071</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>9072</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>9073</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>9074</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>9075</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>9076</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>9077</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>9078</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>9079</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>9080</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>9081</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>9082</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>9083</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>9084</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>9085</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>9086</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>9087</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>9088</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>9089</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>9090</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>9091</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>9092</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>9093</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>9094</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>9095</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>9096</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>9097</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>9098</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>9099</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>9100</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>9101</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>9102</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>9103</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>9104</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>9105</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>9106</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>9107</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>9108</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>9109</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>9110</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>9111</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>9112</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>9113</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>9114</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>9115</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>9116</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>9117</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>9118</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>9119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>9120</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>9121</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>9122</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>9123</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>9124</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>9125</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>9126</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>9127</v>
       </c>
     </row>
   </sheetData>
@@ -40271,7 +40285,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="A2:B66 B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -40307,7 +40321,7 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E46" activeCellId="0" sqref="E46"/>
+      <selection pane="topLeft" activeCell="E46" activeCellId="2" sqref="A2:B66 B66 E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42249,7 +42263,7 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="A2:B66 B66 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43085,7 +43099,7 @@
   <dimension ref="A1:B112"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="2" sqref="A2:B66 B66 D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -44009,7 +44023,7 @@
   <dimension ref="A1:B1039"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="2" sqref="A2:B66 B66 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -52349,7 +52363,7 @@
   <dimension ref="A1:B1803"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="A2:B66 B66 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -66801,7 +66815,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="A2:B66 B66 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -67029,7 +67043,7 @@
   <dimension ref="A1:B179"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B179" activeCellId="0" sqref="B179"/>
+      <selection pane="topLeft" activeCell="B179" activeCellId="2" sqref="A2:B66 B66 B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>